<commit_message>
adjusted selectivity values based on p star method
</commit_message>
<xml_diff>
--- a/rec_selectivity_by_state_cdf_star_raw_18_19.xlsx
+++ b/rec_selectivity_by_state_cdf_star_raw_18_19.xlsx
@@ -147,13 +147,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>6775.80322265625</v>
+        <v>7382.95458984375</v>
       </c>
       <c r="D3" s="2">
         <v>413071</v>
       </c>
       <c r="E3" s="1">
-        <v>8.9413670911753229e-10</v>
+        <v>9.7425656431227026e-10</v>
       </c>
     </row>
     <row r="4">
@@ -164,13 +164,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>8711.74609375</v>
+        <v>9492.3701171875</v>
       </c>
       <c r="D4" s="2">
         <v>413071</v>
       </c>
       <c r="E4" s="1">
-        <v>1.0151249840717469e-09</v>
+        <v>1.1060862226131007e-09</v>
       </c>
     </row>
     <row r="5">
@@ -181,13 +181,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="1">
-        <v>19359.439453125</v>
+        <v>21094.158203125</v>
       </c>
       <c r="D5" s="2">
         <v>413071</v>
       </c>
       <c r="E5" s="1">
-        <v>5.763548749371239e-09</v>
+        <v>6.2799960787174314e-09</v>
       </c>
     </row>
     <row r="6">
@@ -198,13 +198,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="1">
-        <v>14519.578125</v>
+        <v>15820.6162109375</v>
       </c>
       <c r="D6" s="2">
         <v>413071</v>
       </c>
       <c r="E6" s="1">
-        <v>4.4976569135712907e-09</v>
+        <v>4.9006727564915309e-09</v>
       </c>
     </row>
     <row r="7">
@@ -215,13 +215,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="1">
-        <v>48398.59375</v>
+        <v>52735.390625</v>
       </c>
       <c r="D7" s="2">
         <v>413071</v>
       </c>
       <c r="E7" s="1">
-        <v>2.0254264043728654e-08</v>
+        <v>2.206916605018705e-08</v>
       </c>
     </row>
     <row r="8">
@@ -232,13 +232,13 @@
         <v>2</v>
       </c>
       <c r="C8" s="1">
-        <v>121995.65625</v>
+        <v>132927.171875</v>
       </c>
       <c r="D8" s="2">
         <v>413071</v>
       </c>
       <c r="E8" s="1">
-        <v>3.795160097297412e-08</v>
+        <v>4.1352283375317711e-08</v>
       </c>
     </row>
     <row r="9">
@@ -249,13 +249,13 @@
         <v>2</v>
       </c>
       <c r="C9" s="1">
-        <v>126466.21875</v>
+        <v>137798.328125</v>
       </c>
       <c r="D9" s="2">
         <v>413071</v>
       </c>
       <c r="E9" s="1">
-        <v>2.9284816349672838e-08</v>
+        <v>3.1908907516253748e-08</v>
       </c>
     </row>
     <row r="10">
@@ -266,13 +266,13 @@
         <v>2</v>
       </c>
       <c r="C10" s="1">
-        <v>125661.7265625</v>
+        <v>136921.75</v>
       </c>
       <c r="D10" s="2">
         <v>413071</v>
       </c>
       <c r="E10" s="1">
-        <v>1.6754983178657312e-08</v>
+        <v>1.8256328004895295e-08</v>
       </c>
     </row>
     <row r="11">
@@ -283,13 +283,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1">
-        <v>174534.90625</v>
+        <v>190174.25</v>
       </c>
       <c r="D11" s="2">
         <v>413071</v>
       </c>
       <c r="E11" s="1">
-        <v>4.7586592444304188e-08</v>
+        <v>5.1850630455874125e-08</v>
       </c>
     </row>
     <row r="12">
@@ -300,13 +300,13 @@
         <v>2</v>
       </c>
       <c r="C12" s="1">
-        <v>181199.875</v>
+        <v>197436.4375</v>
       </c>
       <c r="D12" s="2">
         <v>413071</v>
       </c>
       <c r="E12" s="1">
-        <v>5.4213828093452321e-08</v>
+        <v>5.9071702196433762e-08</v>
       </c>
     </row>
     <row r="13">
@@ -317,13 +317,13 @@
         <v>2</v>
       </c>
       <c r="C13" s="1">
-        <v>147800.8125</v>
+        <v>161044.625</v>
       </c>
       <c r="D13" s="2">
         <v>413071</v>
       </c>
       <c r="E13" s="1">
-        <v>7.7530032172035135e-08</v>
+        <v>8.4477179029818217e-08</v>
       </c>
     </row>
     <row r="14">
@@ -334,13 +334,13 @@
         <v>2</v>
       </c>
       <c r="C14" s="1">
-        <v>87403.6953125</v>
+        <v>41829.15625</v>
       </c>
       <c r="D14" s="2">
         <v>413071</v>
       </c>
       <c r="E14" s="1">
-        <v>4.7884686438237622e-08</v>
+        <v>2.2916378128456927e-08</v>
       </c>
     </row>
     <row r="15">
@@ -351,13 +351,13 @@
         <v>2</v>
       </c>
       <c r="C15" s="1">
-        <v>32676.037109375</v>
+        <v>17886.884765625</v>
       </c>
       <c r="D15" s="2">
         <v>413071</v>
       </c>
       <c r="E15" s="1">
-        <v>2.1845465880687698e-08</v>
+        <v>1.1958222856378597e-08</v>
       </c>
     </row>
     <row r="16">
@@ -368,13 +368,13 @@
         <v>2</v>
       </c>
       <c r="C16" s="1">
-        <v>26671.0234375</v>
+        <v>14599.7353515625</v>
       </c>
       <c r="D16" s="2">
         <v>413071</v>
       </c>
       <c r="E16" s="1">
-        <v>3.3306665869758945e-08</v>
+        <v>1.8232091392178518e-08</v>
       </c>
     </row>
     <row r="17">
@@ -385,13 +385,13 @@
         <v>2</v>
       </c>
       <c r="C17" s="1">
-        <v>15622.291015625</v>
+        <v>8551.65234375</v>
       </c>
       <c r="D17" s="2">
         <v>413071</v>
       </c>
       <c r="E17" s="1">
-        <v>1.3945946619742244e-08</v>
+        <v>7.6340205268365935e-09</v>
       </c>
     </row>
     <row r="18">
@@ -402,13 +402,13 @@
         <v>2</v>
       </c>
       <c r="C18" s="1">
-        <v>8966.5595703125</v>
+        <v>4908.30029296875</v>
       </c>
       <c r="D18" s="2">
         <v>413071</v>
       </c>
       <c r="E18" s="1">
-        <v>1.1269772670630118e-08</v>
+        <v>6.1690808017544896e-09</v>
       </c>
     </row>
     <row r="19">
@@ -419,13 +419,13 @@
         <v>2</v>
       </c>
       <c r="C19" s="1">
-        <v>5798.63427734375</v>
+        <v>3174.176025390625</v>
       </c>
       <c r="D19" s="2">
         <v>413071</v>
       </c>
       <c r="E19" s="1">
-        <v>7.0738352953014783e-09</v>
+        <v>3.8722216544329058e-09</v>
       </c>
     </row>
     <row r="20">
@@ -436,13 +436,13 @@
         <v>2</v>
       </c>
       <c r="C20" s="1">
-        <v>990.91888427734375</v>
+        <v>542.42962646484375</v>
       </c>
       <c r="D20" s="2">
         <v>413071</v>
       </c>
       <c r="E20" s="1">
-        <v>2.6492272819922391e-09</v>
+        <v>1.4501887468654218e-09</v>
       </c>
     </row>
     <row r="21">
@@ -453,13 +453,13 @@
         <v>2</v>
       </c>
       <c r="C21" s="1">
-        <v>237.30403137207031</v>
+        <v>129.90037536621094</v>
       </c>
       <c r="D21" s="2">
         <v>413071</v>
       </c>
       <c r="E21" s="1">
-        <v>6.285263420835463e-10</v>
+        <v>3.4405570059625745e-10</v>
       </c>
     </row>
     <row r="22">
@@ -470,13 +470,13 @@
         <v>2</v>
       </c>
       <c r="C22" s="1">
-        <v>536.59222412109375</v>
+        <v>293.73092651367188</v>
       </c>
       <c r="D22" s="2">
         <v>413071</v>
       </c>
       <c r="E22" s="1">
-        <v>3.0948044127399044e-09</v>
+        <v>1.694097861992816e-09</v>
       </c>
     </row>
     <row r="23">
@@ -487,13 +487,13 @@
         <v>2</v>
       </c>
       <c r="C23" s="1">
-        <v>857.25408935546875</v>
+        <v>469.26144409179688</v>
       </c>
       <c r="D23" s="2">
         <v>413071</v>
       </c>
       <c r="E23" s="1">
-        <v>4.8831823029615862e-09</v>
+        <v>2.6730571089927935e-09</v>
       </c>
     </row>
     <row r="24">
@@ -521,13 +521,13 @@
         <v>2</v>
       </c>
       <c r="C25" s="1">
-        <v>63.216667175292969</v>
+        <v>34.604843139648438</v>
       </c>
       <c r="D25" s="2">
         <v>413071</v>
       </c>
       <c r="E25" s="1">
-        <v>2.6785138551588261e-09</v>
+        <v>1.4662201452964041e-09</v>
       </c>
     </row>
     <row r="26">
@@ -572,13 +572,13 @@
         <v>3</v>
       </c>
       <c r="C28" s="1">
-        <v>3979.85302734375</v>
+        <v>4528.67431640625</v>
       </c>
       <c r="D28" s="2">
         <v>401288</v>
       </c>
       <c r="E28" s="1">
-        <v>5.4060328436023042e-10</v>
+        <v>6.1515242899545797e-10</v>
       </c>
     </row>
     <row r="29">
@@ -589,13 +589,13 @@
         <v>3</v>
       </c>
       <c r="C29" s="1">
-        <v>5969.779296875</v>
+        <v>6793.01123046875</v>
       </c>
       <c r="D29" s="2">
         <v>401288</v>
       </c>
       <c r="E29" s="1">
-        <v>7.1604633333777201e-10</v>
+        <v>8.1478906954757235e-10</v>
       </c>
     </row>
     <row r="30">
@@ -606,13 +606,13 @@
         <v>3</v>
       </c>
       <c r="C30" s="1">
-        <v>11939.8681640625</v>
+        <v>13586.3740234375</v>
       </c>
       <c r="D30" s="2">
         <v>401288</v>
       </c>
       <c r="E30" s="1">
-        <v>3.6590239727019025e-09</v>
+        <v>4.1636027958702471e-09</v>
       </c>
     </row>
     <row r="31">
@@ -623,13 +623,13 @@
         <v>3</v>
       </c>
       <c r="C31" s="1">
-        <v>23879.921875</v>
+        <v>27172.9609375</v>
       </c>
       <c r="D31" s="2">
         <v>401288</v>
       </c>
       <c r="E31" s="1">
-        <v>7.6143660265870494e-09</v>
+        <v>8.6643865415680921e-09</v>
       </c>
     </row>
     <row r="32">
@@ -640,13 +640,13 @@
         <v>3</v>
       </c>
       <c r="C32" s="1">
-        <v>45768.3125</v>
+        <v>52079.75390625</v>
       </c>
       <c r="D32" s="2">
         <v>401288</v>
       </c>
       <c r="E32" s="1">
-        <v>1.9715924892693693e-08</v>
+        <v>2.2434747393162979e-08</v>
       </c>
     </row>
     <row r="33">
@@ -657,13 +657,13 @@
         <v>3</v>
       </c>
       <c r="C33" s="1">
-        <v>77610.2578125</v>
+        <v>88312.703125</v>
       </c>
       <c r="D33" s="2">
         <v>401288</v>
       </c>
       <c r="E33" s="1">
-        <v>2.4852688795817812e-08</v>
+        <v>2.8279872665848416e-08</v>
       </c>
     </row>
     <row r="34">
@@ -674,13 +674,13 @@
         <v>3</v>
       </c>
       <c r="C34" s="1">
-        <v>117786.9765625</v>
+        <v>134029.78125</v>
       </c>
       <c r="D34" s="2">
         <v>401288</v>
       </c>
       <c r="E34" s="1">
-        <v>2.8075906044477961e-08</v>
+        <v>3.1947568146506455e-08</v>
       </c>
     </row>
     <row r="35">
@@ -691,13 +691,13 @@
         <v>3</v>
       </c>
       <c r="C35" s="1">
-        <v>118327.9453125</v>
+        <v>135233.75</v>
       </c>
       <c r="D35" s="2">
         <v>401288</v>
       </c>
       <c r="E35" s="1">
-        <v>1.6240404576706169e-08</v>
+        <v>1.8560710302040206e-08</v>
       </c>
     </row>
     <row r="36">
@@ -708,13 +708,13 @@
         <v>3</v>
       </c>
       <c r="C36" s="1">
-        <v>56474.09765625</v>
+        <v>29260.83203125</v>
       </c>
       <c r="D36" s="2">
         <v>401288</v>
       </c>
       <c r="E36" s="1">
-        <v>1.5849668244527493e-08</v>
+        <v>8.212162505571996e-09</v>
       </c>
     </row>
     <row r="37">
@@ -725,13 +725,13 @@
         <v>3</v>
       </c>
       <c r="C37" s="1">
-        <v>26512.328125</v>
+        <v>14851.013671875</v>
       </c>
       <c r="D37" s="2">
         <v>401288</v>
       </c>
       <c r="E37" s="1">
-        <v>8.1652329342318808e-09</v>
+        <v>4.573796008600084e-09</v>
       </c>
     </row>
     <row r="38">
@@ -742,13 +742,13 @@
         <v>3</v>
       </c>
       <c r="C38" s="1">
-        <v>19543.951171875</v>
+        <v>10947.6416015625</v>
       </c>
       <c r="D38" s="2">
         <v>401288</v>
       </c>
       <c r="E38" s="1">
-        <v>1.0552954066156417e-08</v>
+        <v>5.9112901240609972e-09</v>
       </c>
     </row>
     <row r="39">
@@ -759,13 +759,13 @@
         <v>3</v>
       </c>
       <c r="C39" s="1">
-        <v>10862.0146484375</v>
+        <v>6084.41162109375</v>
       </c>
       <c r="D39" s="2">
         <v>401288</v>
       </c>
       <c r="E39" s="1">
-        <v>6.1255596150999736e-09</v>
+        <v>3.4312628294230763e-09</v>
       </c>
     </row>
     <row r="40">
@@ -776,13 +776,13 @@
         <v>3</v>
       </c>
       <c r="C40" s="1">
-        <v>3729.3203125</v>
+        <v>2088.99755859375</v>
       </c>
       <c r="D40" s="2">
         <v>401288</v>
       </c>
       <c r="E40" s="1">
-        <v>2.5664343983322624e-09</v>
+        <v>1.4376011492345242e-09</v>
       </c>
     </row>
     <row r="41">
@@ -793,13 +793,13 @@
         <v>3</v>
       </c>
       <c r="C41" s="1">
-        <v>1345.5067138671875</v>
+        <v>753.69232177734375</v>
       </c>
       <c r="D41" s="2">
         <v>401288</v>
       </c>
       <c r="E41" s="1">
-        <v>1.7296009069411866e-09</v>
+        <v>9.6884456013413001e-10</v>
       </c>
     </row>
     <row r="42">
@@ -810,13 +810,13 @@
         <v>3</v>
       </c>
       <c r="C42" s="1">
-        <v>3192.2021484375</v>
+        <v>1788.1279296875</v>
       </c>
       <c r="D42" s="2">
         <v>401288</v>
       </c>
       <c r="E42" s="1">
-        <v>2.9333384610197299e-09</v>
+        <v>1.6431241922632012e-09</v>
       </c>
     </row>
     <row r="43">
@@ -827,13 +827,13 @@
         <v>3</v>
       </c>
       <c r="C43" s="1">
-        <v>25.691064834594727</v>
+        <v>14.390978813171387</v>
       </c>
       <c r="D43" s="2">
         <v>401288</v>
       </c>
       <c r="E43" s="1">
-        <v>3.3238387736611585e-11</v>
+        <v>1.8618650024504468e-11</v>
       </c>
     </row>
     <row r="44">
@@ -844,13 +844,13 @@
         <v>3</v>
       </c>
       <c r="C44" s="1">
-        <v>254.52424621582031</v>
+        <v>142.57302856445313</v>
       </c>
       <c r="D44" s="2">
         <v>401288</v>
       </c>
       <c r="E44" s="1">
-        <v>3.1961480684294941e-10</v>
+        <v>1.7903384330608674e-10</v>
       </c>
     </row>
     <row r="45">
@@ -861,13 +861,13 @@
         <v>3</v>
       </c>
       <c r="C45" s="1">
-        <v>178.62748718261719</v>
+        <v>100.05908203125</v>
       </c>
       <c r="D45" s="2">
         <v>401288</v>
       </c>
       <c r="E45" s="1">
-        <v>4.9158421777661943e-10</v>
+        <v>2.7536337099398622e-10</v>
       </c>
     </row>
     <row r="46">
@@ -878,13 +878,13 @@
         <v>3</v>
       </c>
       <c r="C46" s="1">
-        <v>881.1624755859375</v>
+        <v>493.58755493164063</v>
       </c>
       <c r="D46" s="2">
         <v>401288</v>
       </c>
       <c r="E46" s="1">
-        <v>2.4023865119460197e-09</v>
+        <v>1.3457087666424172e-09</v>
       </c>
     </row>
     <row r="47">
@@ -1014,13 +1014,13 @@
         <v>4</v>
       </c>
       <c r="C54" s="1">
-        <v>6398.80419921875</v>
+        <v>9238.4013671875</v>
       </c>
       <c r="D54" s="2">
         <v>104251</v>
       </c>
       <c r="E54" s="1">
-        <v>7.548149660863146e-09</v>
+        <v>1.089779111396183e-08</v>
       </c>
     </row>
     <row r="55">
@@ -1031,13 +1031,13 @@
         <v>4</v>
       </c>
       <c r="C55" s="1">
-        <v>6398.80419921875</v>
+        <v>9238.4013671875</v>
       </c>
       <c r="D55" s="2">
         <v>104251</v>
       </c>
       <c r="E55" s="1">
-        <v>7.8537238934472953e-09</v>
+        <v>1.1338970651308955e-08</v>
       </c>
     </row>
     <row r="56">
@@ -1048,13 +1048,13 @@
         <v>4</v>
       </c>
       <c r="C56" s="1">
-        <v>12797.6083984375</v>
+        <v>18476.802734375</v>
       </c>
       <c r="D56" s="2">
         <v>104251</v>
       </c>
       <c r="E56" s="1">
-        <v>2.1220570189939281e-08</v>
+        <v>3.0637622217000171e-08</v>
       </c>
     </row>
     <row r="57">
@@ -1065,13 +1065,13 @@
         <v>4</v>
       </c>
       <c r="C57" s="1">
-        <v>25925.83984375</v>
+        <v>37430.94921875</v>
       </c>
       <c r="D57" s="2">
         <v>104251</v>
       </c>
       <c r="E57" s="1">
-        <v>3.1956780333075585e-08</v>
+        <v>4.6138243448012872e-08</v>
       </c>
     </row>
     <row r="58">
@@ -1082,13 +1082,13 @@
         <v>4</v>
       </c>
       <c r="C58" s="1">
-        <v>18770.712890625</v>
+        <v>27100.591796875</v>
       </c>
       <c r="D58" s="2">
         <v>104251</v>
       </c>
       <c r="E58" s="1">
-        <v>1.7222381742953985e-08</v>
+        <v>2.4865158820830402e-08</v>
       </c>
     </row>
     <row r="59">
@@ -1099,13 +1099,13 @@
         <v>4</v>
       </c>
       <c r="C59" s="1">
-        <v>19475.2890625</v>
+        <v>28117.837890625</v>
       </c>
       <c r="D59" s="2">
         <v>104251</v>
       </c>
       <c r="E59" s="1">
-        <v>1.0288910168299026e-08</v>
+        <v>1.4854819596621383e-08</v>
       </c>
     </row>
     <row r="60">
@@ -1116,13 +1116,13 @@
         <v>4</v>
       </c>
       <c r="C60" s="1">
-        <v>67213.2890625</v>
+        <v>97040.53125</v>
       </c>
       <c r="D60" s="2">
         <v>104251</v>
       </c>
       <c r="E60" s="1">
-        <v>7.2610923496085888e-08</v>
+        <v>1.0483346812861782e-07</v>
       </c>
     </row>
     <row r="61">
@@ -1133,13 +1133,13 @@
         <v>4</v>
       </c>
       <c r="C61" s="1">
-        <v>69663.171875</v>
+        <v>16215.6904296875</v>
       </c>
       <c r="D61" s="2">
         <v>104251</v>
       </c>
       <c r="E61" s="1">
-        <v>8.2584755034531554e-08</v>
+        <v>1.9223483249675155e-08</v>
       </c>
     </row>
     <row r="62">
@@ -1150,13 +1150,13 @@
         <v>4</v>
       </c>
       <c r="C62" s="1">
-        <v>14914.666015625</v>
+        <v>10365.4443359375</v>
       </c>
       <c r="D62" s="2">
         <v>104251</v>
       </c>
       <c r="E62" s="1">
-        <v>3.0999249389651595e-08</v>
+        <v>2.1543961281622614e-08</v>
       </c>
     </row>
     <row r="63">
@@ -1167,13 +1167,13 @@
         <v>4</v>
       </c>
       <c r="C63" s="1">
-        <v>8330.8525390625</v>
+        <v>5789.8037109375</v>
       </c>
       <c r="D63" s="2">
         <v>104251</v>
       </c>
       <c r="E63" s="1">
-        <v>1.8084261199646789e-08</v>
+        <v>1.2568261098522271e-08</v>
       </c>
     </row>
     <row r="64">
@@ -1184,13 +1184,13 @@
         <v>4</v>
       </c>
       <c r="C64" s="1">
-        <v>15416.486328125</v>
+        <v>10714.201171875</v>
       </c>
       <c r="D64" s="2">
         <v>104251</v>
       </c>
       <c r="E64" s="1">
-        <v>4.0837750958644392e-08</v>
+        <v>2.8381556660406204e-08</v>
       </c>
     </row>
     <row r="65">
@@ -1201,13 +1201,13 @@
         <v>4</v>
       </c>
       <c r="C65" s="1">
-        <v>5477.11962890625</v>
+        <v>3806.5068359375</v>
       </c>
       <c r="D65" s="2">
         <v>104251</v>
       </c>
       <c r="E65" s="1">
-        <v>2.7101179966848576e-08</v>
+        <v>1.8834867887562723e-08</v>
       </c>
     </row>
     <row r="66">
@@ -1218,13 +1218,13 @@
         <v>4</v>
       </c>
       <c r="C66" s="1">
-        <v>4661.189453125</v>
+        <v>3239.448974609375</v>
       </c>
       <c r="D66" s="2">
         <v>104251</v>
       </c>
       <c r="E66" s="1">
-        <v>1.6487108567275754e-08</v>
+        <v>1.1458265447572558e-08</v>
       </c>
     </row>
     <row r="67">
@@ -1235,13 +1235,13 @@
         <v>4</v>
       </c>
       <c r="C67" s="1">
-        <v>3570.402099609375</v>
+        <v>2481.369873046875</v>
       </c>
       <c r="D67" s="2">
         <v>104251</v>
       </c>
       <c r="E67" s="1">
-        <v>1.7780784844489972e-08</v>
+        <v>1.2357348921909761e-08</v>
       </c>
     </row>
     <row r="68">
@@ -1252,13 +1252,13 @@
         <v>4</v>
       </c>
       <c r="C68" s="1">
-        <v>715.3070068359375</v>
+        <v>497.12643432617188</v>
       </c>
       <c r="D68" s="2">
         <v>104251</v>
       </c>
       <c r="E68" s="1">
-        <v>3.4575318164087321e-09</v>
+        <v>2.4029267464698023e-09</v>
       </c>
     </row>
     <row r="69">
@@ -1303,13 +1303,13 @@
         <v>4</v>
       </c>
       <c r="C71" s="1">
-        <v>77.271942138671875</v>
+        <v>53.702713012695313</v>
       </c>
       <c r="D71" s="2">
         <v>104251</v>
       </c>
       <c r="E71" s="1">
-        <v>1.7658553508326236e-09</v>
+        <v>1.2272400873314382e-09</v>
       </c>
     </row>
     <row r="72">
@@ -1388,13 +1388,13 @@
         <v>5</v>
       </c>
       <c r="C76" s="1">
-        <v>29103.9921875</v>
+        <v>30085.1767578125</v>
       </c>
       <c r="D76" s="2">
         <v>544681</v>
       </c>
       <c r="E76" s="1">
-        <v>4.3031484153743804e-08</v>
+        <v>4.4482206362772558e-08</v>
       </c>
     </row>
     <row r="77">
@@ -1405,13 +1405,13 @@
         <v>5</v>
       </c>
       <c r="C77" s="1">
-        <v>50032.640625</v>
+        <v>51899.96875</v>
       </c>
       <c r="D77" s="2">
         <v>544681</v>
       </c>
       <c r="E77" s="1">
-        <v>6.0268301460553175e-09</v>
+        <v>6.251764883558053e-09</v>
       </c>
     </row>
     <row r="78">
@@ -1422,13 +1422,13 @@
         <v>5</v>
       </c>
       <c r="C78" s="1">
-        <v>55395.890625</v>
+        <v>57463.38671875</v>
       </c>
       <c r="D78" s="2">
         <v>544681</v>
       </c>
       <c r="E78" s="1">
-        <v>5.5437436863314815e-09</v>
+        <v>5.7506484019143045e-09</v>
       </c>
     </row>
     <row r="79">
@@ -1439,13 +1439,13 @@
         <v>5</v>
       </c>
       <c r="C79" s="1">
-        <v>71883.3828125</v>
+        <v>74566.2265625</v>
       </c>
       <c r="D79" s="2">
         <v>544681</v>
       </c>
       <c r="E79" s="1">
-        <v>6.3522169746477175e-09</v>
+        <v>6.589295331593803e-09</v>
       </c>
     </row>
     <row r="80">
@@ -1456,13 +1456,13 @@
         <v>5</v>
       </c>
       <c r="C80" s="1">
-        <v>128631.1328125</v>
+        <v>133431.9375</v>
       </c>
       <c r="D80" s="2">
         <v>544681</v>
       </c>
       <c r="E80" s="1">
-        <v>2.9041949289876356e-08</v>
+        <v>3.0125860916996317e-08</v>
       </c>
     </row>
     <row r="81">
@@ -1473,13 +1473,13 @@
         <v>5</v>
       </c>
       <c r="C81" s="1">
-        <v>223461.390625</v>
+        <v>231801.453125</v>
       </c>
       <c r="D81" s="2">
         <v>544681</v>
       </c>
       <c r="E81" s="1">
-        <v>5.2494922186951953e-08</v>
+        <v>5.4454144304827423e-08</v>
       </c>
     </row>
     <row r="82">
@@ -1490,13 +1490,13 @@
         <v>5</v>
       </c>
       <c r="C82" s="1">
-        <v>140919.203125</v>
+        <v>146178.609375</v>
       </c>
       <c r="D82" s="2">
         <v>544681</v>
       </c>
       <c r="E82" s="1">
-        <v>4.4723563519255549e-08</v>
+        <v>4.6392742092393746e-08</v>
       </c>
     </row>
     <row r="83">
@@ -1507,13 +1507,13 @@
         <v>5</v>
       </c>
       <c r="C83" s="1">
-        <v>76175.546875</v>
+        <v>79018.5859375</v>
       </c>
       <c r="D83" s="2">
         <v>544681</v>
       </c>
       <c r="E83" s="1">
-        <v>1.7971478527556428e-08</v>
+        <v>1.8642213106545569e-08</v>
       </c>
     </row>
     <row r="84">
@@ -1524,13 +1524,13 @@
         <v>5</v>
       </c>
       <c r="C84" s="1">
-        <v>61683.2578125</v>
+        <v>63985.4140625</v>
       </c>
       <c r="D84" s="2">
         <v>544681</v>
       </c>
       <c r="E84" s="1">
-        <v>1.0832227559376406e-08</v>
+        <v>1.1236510388812349e-08</v>
       </c>
     </row>
     <row r="85">
@@ -1541,13 +1541,13 @@
         <v>5</v>
       </c>
       <c r="C85" s="1">
-        <v>65187.88671875</v>
+        <v>67728.296875</v>
       </c>
       <c r="D85" s="2">
         <v>544681</v>
       </c>
       <c r="E85" s="1">
-        <v>6.5915926050763574e-09</v>
+        <v>6.8484711235328177e-09</v>
       </c>
     </row>
     <row r="86">
@@ -1558,13 +1558,13 @@
         <v>5</v>
       </c>
       <c r="C86" s="1">
-        <v>33684.73828125</v>
+        <v>23651.900390625</v>
       </c>
       <c r="D86" s="2">
         <v>544681</v>
       </c>
       <c r="E86" s="1">
-        <v>6.9649495060275513e-09</v>
+        <v>4.8904729155196947e-09</v>
       </c>
     </row>
     <row r="87">
@@ -1575,13 +1575,13 @@
         <v>5</v>
       </c>
       <c r="C87" s="1">
-        <v>33559.91015625</v>
+        <v>23809.2265625</v>
       </c>
       <c r="D87" s="2">
         <v>544681</v>
       </c>
       <c r="E87" s="1">
-        <v>7.6147461669506811e-09</v>
+        <v>5.4023154838489518e-09</v>
       </c>
     </row>
     <row r="88">
@@ -1592,13 +1592,13 @@
         <v>5</v>
       </c>
       <c r="C88" s="1">
-        <v>17296.1953125</v>
+        <v>12270.8623046875</v>
       </c>
       <c r="D88" s="2">
         <v>544681</v>
       </c>
       <c r="E88" s="1">
-        <v>6.8805987574194205e-09</v>
+        <v>4.8814712272360339e-09</v>
       </c>
     </row>
     <row r="89">
@@ -1609,13 +1609,13 @@
         <v>5</v>
       </c>
       <c r="C89" s="1">
-        <v>17406.576171875</v>
+        <v>12349.173828125</v>
       </c>
       <c r="D89" s="2">
         <v>544681</v>
       </c>
       <c r="E89" s="1">
-        <v>7.2320713861984132e-09</v>
+        <v>5.1308255422100046e-09</v>
       </c>
     </row>
     <row r="90">
@@ -1626,13 +1626,13 @@
         <v>5</v>
       </c>
       <c r="C90" s="1">
-        <v>8982.533203125</v>
+        <v>6372.69775390625</v>
       </c>
       <c r="D90" s="2">
         <v>544681</v>
       </c>
       <c r="E90" s="1">
-        <v>4.554212118534906e-09</v>
+        <v>3.2310059072671038e-09</v>
       </c>
     </row>
     <row r="91">
@@ -1643,13 +1643,13 @@
         <v>5</v>
       </c>
       <c r="C91" s="1">
-        <v>1941.474365234375</v>
+        <v>1377.3875732421875</v>
       </c>
       <c r="D91" s="2">
         <v>544681</v>
       </c>
       <c r="E91" s="1">
-        <v>1.8386778766199541e-09</v>
+        <v>1.3044580970955622e-09</v>
       </c>
     </row>
     <row r="92">
@@ -1660,13 +1660,13 @@
         <v>5</v>
       </c>
       <c r="C92" s="1">
-        <v>1389.294921875</v>
+        <v>985.64141845703125</v>
       </c>
       <c r="D92" s="2">
         <v>544681</v>
       </c>
       <c r="E92" s="1">
-        <v>9.4054630750406432e-10</v>
+        <v>6.6727473546634997e-10</v>
       </c>
     </row>
     <row r="93">
@@ -1677,13 +1677,13 @@
         <v>5</v>
       </c>
       <c r="C93" s="1">
-        <v>251.79917907714844</v>
+        <v>178.64004516601563</v>
       </c>
       <c r="D93" s="2">
         <v>544681</v>
       </c>
       <c r="E93" s="1">
-        <v>2.4000823550807127e-10</v>
+        <v>1.7027490528676026e-10</v>
       </c>
     </row>
     <row r="94">
@@ -1711,13 +1711,13 @@
         <v>5</v>
       </c>
       <c r="C95" s="1">
-        <v>1.5880948305130005</v>
+        <v>1.1266809701919556</v>
       </c>
       <c r="D95" s="2">
         <v>544681</v>
       </c>
       <c r="E95" s="1">
-        <v>3.2198824769652523e-12</v>
+        <v>2.2843599841587681e-12</v>
       </c>
     </row>
     <row r="96">
@@ -1728,13 +1728,13 @@
         <v>5</v>
       </c>
       <c r="C96" s="1">
-        <v>575.76568603515625</v>
+        <v>408.47952270507813</v>
       </c>
       <c r="D96" s="2">
         <v>544681</v>
       </c>
       <c r="E96" s="1">
-        <v>1.1565025603843537e-09</v>
+        <v>8.2048590144268019e-10</v>
       </c>
     </row>
     <row r="97">
@@ -1830,13 +1830,13 @@
         <v>6</v>
       </c>
       <c r="C102" s="1">
-        <v>174.72308731079102</v>
+        <v>180.49602699279785</v>
       </c>
       <c r="D102" s="2">
         <v>26646</v>
       </c>
       <c r="E102" s="1">
-        <v>5.2807336281546213e-09</v>
+        <v>5.4552118378126124e-09</v>
       </c>
     </row>
     <row r="103">
@@ -1847,13 +1847,13 @@
         <v>6</v>
       </c>
       <c r="C103" s="1">
-        <v>141.11566162109375</v>
+        <v>152.10235595703125</v>
       </c>
       <c r="D103" s="2">
         <v>26646</v>
       </c>
       <c r="E103" s="1">
-        <v>3.4747291155490245e-10</v>
+        <v>3.7452574375151926e-10</v>
       </c>
     </row>
     <row r="104">
@@ -1864,13 +1864,13 @@
         <v>6</v>
       </c>
       <c r="C104" s="1">
-        <v>156.2425537109375</v>
+        <v>168.40696716308594</v>
       </c>
       <c r="D104" s="2">
         <v>26646</v>
       </c>
       <c r="E104" s="1">
-        <v>3.1962088531400923e-10</v>
+        <v>3.4450525765450379e-10</v>
       </c>
     </row>
     <row r="105">
@@ -1881,13 +1881,13 @@
         <v>6</v>
       </c>
       <c r="C105" s="1">
-        <v>202.74505615234375</v>
+        <v>218.52995300292969</v>
       </c>
       <c r="D105" s="2">
         <v>26646</v>
       </c>
       <c r="E105" s="1">
-        <v>3.662328496023548e-10</v>
+        <v>3.9474620794344162e-10</v>
       </c>
     </row>
     <row r="106">
@@ -1898,13 +1898,13 @@
         <v>6</v>
       </c>
       <c r="C106" s="1">
-        <v>362.80050659179688</v>
+        <v>391.04666137695313</v>
       </c>
       <c r="D106" s="2">
         <v>26646</v>
       </c>
       <c r="E106" s="1">
-        <v>1.6743944009078859e-09</v>
+        <v>1.8047557892586497e-09</v>
       </c>
     </row>
     <row r="107">
@@ -1915,13 +1915,13 @@
         <v>6</v>
       </c>
       <c r="C107" s="1">
-        <v>630.26654052734375</v>
+        <v>679.3365478515625</v>
       </c>
       <c r="D107" s="2">
         <v>26646</v>
       </c>
       <c r="E107" s="1">
-        <v>3.0265596695500108e-09</v>
+        <v>3.2621954026978983e-09</v>
       </c>
     </row>
     <row r="108">
@@ -1932,13 +1932,13 @@
         <v>6</v>
       </c>
       <c r="C108" s="1">
-        <v>397.45864868164063</v>
+        <v>428.40313720703125</v>
       </c>
       <c r="D108" s="2">
         <v>26646</v>
       </c>
       <c r="E108" s="1">
-        <v>2.5785074075912462e-09</v>
+        <v>2.7792592671715965e-09</v>
       </c>
     </row>
     <row r="109">
@@ -1949,13 +1949,13 @@
         <v>6</v>
       </c>
       <c r="C109" s="1">
-        <v>214.85099792480469</v>
+        <v>231.57841491699219</v>
       </c>
       <c r="D109" s="2">
         <v>26646</v>
       </c>
       <c r="E109" s="1">
-        <v>1.0361336233444263e-09</v>
+        <v>1.1168027613805975e-09</v>
       </c>
     </row>
     <row r="110">
@@ -1966,13 +1966,13 @@
         <v>6</v>
       </c>
       <c r="C110" s="1">
-        <v>173.97589111328125</v>
+        <v>95.509941101074219</v>
       </c>
       <c r="D110" s="2">
         <v>26646</v>
       </c>
       <c r="E110" s="1">
-        <v>6.2452487625819231e-10</v>
+        <v>3.428540229499788e-10</v>
       </c>
     </row>
     <row r="111">
@@ -1983,13 +1983,13 @@
         <v>6</v>
       </c>
       <c r="C111" s="1">
-        <v>91.231063842773438</v>
+        <v>12171.7392578125</v>
       </c>
       <c r="D111" s="2">
         <v>26646</v>
       </c>
       <c r="E111" s="1">
-        <v>1.8857165828833899e-10</v>
+        <v>2.5158589878060411e-08</v>
       </c>
     </row>
     <row r="112">
@@ -2000,13 +2000,13 @@
         <v>6</v>
       </c>
       <c r="C112" s="1">
-        <v>9825.55078125</v>
+        <v>6289.10595703125</v>
       </c>
       <c r="D112" s="2">
         <v>26646</v>
       </c>
       <c r="E112" s="1">
-        <v>4.1529041538979072e-08</v>
+        <v>2.6581771450651104e-08</v>
       </c>
     </row>
     <row r="113">
@@ -2017,13 +2017,13 @@
         <v>6</v>
       </c>
       <c r="C113" s="1">
-        <v>9890.9072265625</v>
+        <v>6330.93896484375</v>
       </c>
       <c r="D113" s="2">
         <v>26646</v>
       </c>
       <c r="E113" s="1">
-        <v>4.5875516718751896e-08</v>
+        <v>2.9363848241814594e-08</v>
       </c>
     </row>
     <row r="114">
@@ -2034,13 +2034,13 @@
         <v>6</v>
       </c>
       <c r="C114" s="1">
-        <v>5097.60205078125</v>
+        <v>3262.856201171875</v>
       </c>
       <c r="D114" s="2">
         <v>26646</v>
       </c>
       <c r="E114" s="1">
-        <v>4.1452601351466001e-08</v>
+        <v>2.6532841701509824e-08</v>
       </c>
     </row>
     <row r="115">
@@ -2051,13 +2051,13 @@
         <v>6</v>
       </c>
       <c r="C115" s="1">
-        <v>5130.13427734375</v>
+        <v>3283.679443359375</v>
       </c>
       <c r="D115" s="2">
         <v>26646</v>
       </c>
       <c r="E115" s="1">
-        <v>4.3570071994736281e-08</v>
+        <v>2.78881877591175e-08</v>
       </c>
     </row>
     <row r="116">
@@ -2068,13 +2068,13 @@
         <v>6</v>
       </c>
       <c r="C116" s="1">
-        <v>2647.3671875</v>
+        <v>1694.51806640625</v>
       </c>
       <c r="D116" s="2">
         <v>26646</v>
       </c>
       <c r="E116" s="1">
-        <v>2.7437138783170667e-08</v>
+        <v>1.7561873733029643e-08</v>
       </c>
     </row>
     <row r="117">
@@ -2085,13 +2085,13 @@
         <v>6</v>
       </c>
       <c r="C117" s="1">
-        <v>572.19891357421875</v>
+        <v>366.25119018554688</v>
       </c>
       <c r="D117" s="2">
         <v>26646</v>
       </c>
       <c r="E117" s="1">
-        <v>1.1077230688272266e-08</v>
+        <v>7.090277254206967e-09</v>
       </c>
     </row>
     <row r="118">
@@ -2102,13 +2102,13 @@
         <v>6</v>
       </c>
       <c r="C118" s="1">
-        <v>409.45840454101563</v>
+        <v>262.08477783203125</v>
       </c>
       <c r="D118" s="2">
         <v>26646</v>
       </c>
       <c r="E118" s="1">
-        <v>5.6663806979884157e-09</v>
+        <v>3.6269180991865824e-09</v>
       </c>
     </row>
     <row r="119">
@@ -2119,13 +2119,13 @@
         <v>6</v>
       </c>
       <c r="C119" s="1">
-        <v>74.21124267578125</v>
+        <v>47.500885009765625</v>
       </c>
       <c r="D119" s="2">
         <v>26646</v>
       </c>
       <c r="E119" s="1">
-        <v>1.4459448083314896e-09</v>
+        <v>9.2551555308517663e-10</v>
       </c>
     </row>
     <row r="120">
@@ -2153,13 +2153,13 @@
         <v>6</v>
       </c>
       <c r="C121" s="1">
-        <v>0.46804952621459961</v>
+        <v>0.29958760738372803</v>
       </c>
       <c r="D121" s="2">
         <v>26646</v>
       </c>
       <c r="E121" s="1">
-        <v>1.9398385675550855e-11</v>
+        <v>1.2416455884289856e-11</v>
       </c>
     </row>
     <row r="122">
@@ -2170,13 +2170,13 @@
         <v>6</v>
       </c>
       <c r="C122" s="1">
-        <v>169.69190979003906</v>
+        <v>108.61583709716797</v>
       </c>
       <c r="D122" s="2">
         <v>26646</v>
       </c>
       <c r="E122" s="1">
-        <v>6.9674226388372063e-09</v>
+        <v>4.4596850656830611e-09</v>
       </c>
     </row>
     <row r="123">
@@ -2272,13 +2272,13 @@
         <v>7</v>
       </c>
       <c r="C128" s="1">
-        <v>13066.57958984375</v>
+        <v>13443.02294921875</v>
       </c>
       <c r="D128" s="2">
         <v>4579196</v>
       </c>
       <c r="E128" s="1">
-        <v>2.297992907074331e-09</v>
+        <v>2.3641972823895685e-09</v>
       </c>
     </row>
     <row r="129">
@@ -2289,13 +2289,13 @@
         <v>7</v>
       </c>
       <c r="C129" s="1">
-        <v>8589.78515625</v>
+        <v>9091.7099609375</v>
       </c>
       <c r="D129" s="2">
         <v>4579196</v>
       </c>
       <c r="E129" s="1">
-        <v>1.2307527219590497e-10</v>
+        <v>1.3026690837136812e-10</v>
       </c>
     </row>
     <row r="130">
@@ -2306,13 +2306,13 @@
         <v>7</v>
       </c>
       <c r="C130" s="1">
-        <v>17179.5703125</v>
+        <v>18183.419921875</v>
       </c>
       <c r="D130" s="2">
         <v>4579196</v>
       </c>
       <c r="E130" s="1">
-        <v>2.0449886228846026e-10</v>
+        <v>2.1644828984701547e-10</v>
       </c>
     </row>
     <row r="131">
@@ -2323,13 +2323,13 @@
         <v>7</v>
       </c>
       <c r="C131" s="1">
-        <v>64423.390625</v>
+        <v>68187.8203125</v>
       </c>
       <c r="D131" s="2">
         <v>4579196</v>
       </c>
       <c r="E131" s="1">
-        <v>6.7716326990208131e-10</v>
+        <v>7.1673167401087312e-10</v>
       </c>
     </row>
     <row r="132">
@@ -2340,13 +2340,13 @@
         <v>7</v>
       </c>
       <c r="C132" s="1">
-        <v>367213.34375</v>
+        <v>388670.59375</v>
       </c>
       <c r="D132" s="2">
         <v>4579196</v>
       </c>
       <c r="E132" s="1">
-        <v>9.8616848021038095e-09</v>
+        <v>1.0437928743556313e-08</v>
       </c>
     </row>
     <row r="133">
@@ -2357,13 +2357,13 @@
         <v>7</v>
       </c>
       <c r="C133" s="1">
-        <v>842769.375</v>
+        <v>892014.625</v>
       </c>
       <c r="D133" s="2">
         <v>4579196</v>
       </c>
       <c r="E133" s="1">
-        <v>2.3549221239704821e-08</v>
+        <v>2.4925263630848349e-08</v>
       </c>
     </row>
     <row r="134">
@@ -2374,13 +2374,13 @@
         <v>7</v>
       </c>
       <c r="C134" s="1">
-        <v>1580520.5</v>
+        <v>1672874.625</v>
       </c>
       <c r="D134" s="2">
         <v>4579196</v>
       </c>
       <c r="E134" s="1">
-        <v>5.9664955642801942e-08</v>
+        <v>6.3151347262646595e-08</v>
       </c>
     </row>
     <row r="135">
@@ -2391,13 +2391,13 @@
         <v>7</v>
       </c>
       <c r="C135" s="1">
-        <v>1627764.5</v>
+        <v>1722879.25</v>
       </c>
       <c r="D135" s="2">
         <v>4579196</v>
       </c>
       <c r="E135" s="1">
-        <v>4.5678600457677021e-08</v>
+        <v>4.8347725822850407e-08</v>
       </c>
     </row>
     <row r="136">
@@ -2408,13 +2408,13 @@
         <v>7</v>
       </c>
       <c r="C136" s="1">
-        <v>2059598</v>
+        <v>2179945.75</v>
       </c>
       <c r="D136" s="2">
         <v>4579196</v>
       </c>
       <c r="E136" s="1">
-        <v>4.3021536555443163e-08</v>
+        <v>4.553539767471193e-08</v>
       </c>
     </row>
     <row r="137">
@@ -2425,13 +2425,13 @@
         <v>7</v>
       </c>
       <c r="C137" s="1">
-        <v>2028343.375</v>
+        <v>2146865</v>
       </c>
       <c r="D137" s="2">
         <v>4579196</v>
       </c>
       <c r="E137" s="1">
-        <v>2.4395960807055417e-08</v>
+        <v>2.5821483617960439e-08</v>
       </c>
     </row>
     <row r="138">
@@ -2442,13 +2442,13 @@
         <v>7</v>
       </c>
       <c r="C138" s="1">
-        <v>2008967.125</v>
+        <v>2126356.5</v>
       </c>
       <c r="D138" s="2">
         <v>4579196</v>
       </c>
       <c r="E138" s="1">
-        <v>4.9409518254606155e-08</v>
+        <v>5.2296648789251776e-08</v>
       </c>
     </row>
     <row r="139">
@@ -2459,13 +2459,13 @@
         <v>7</v>
       </c>
       <c r="C139" s="1">
-        <v>1703948.5</v>
+        <v>1803709.375</v>
       </c>
       <c r="D139" s="2">
         <v>4579196</v>
       </c>
       <c r="E139" s="1">
-        <v>4.5987956553972253e-08</v>
+        <v>4.8680409037160643e-08</v>
       </c>
     </row>
     <row r="140">
@@ -2476,13 +2476,13 @@
         <v>7</v>
       </c>
       <c r="C140" s="1">
-        <v>719837.6875</v>
+        <v>557451.125</v>
       </c>
       <c r="D140" s="2">
         <v>4579196</v>
       </c>
       <c r="E140" s="1">
-        <v>3.4061457654388505e-08</v>
+        <v>2.6377609430028315e-08</v>
       </c>
     </row>
     <row r="141">
@@ -2493,13 +2493,13 @@
         <v>7</v>
       </c>
       <c r="C141" s="1">
-        <v>437439.59375</v>
+        <v>222423.40625</v>
       </c>
       <c r="D141" s="2">
         <v>4579196</v>
       </c>
       <c r="E141" s="1">
-        <v>2.1618244971932654e-08</v>
+        <v>1.099215474198445e-08</v>
       </c>
     </row>
     <row r="142">
@@ -2510,13 +2510,13 @@
         <v>7</v>
       </c>
       <c r="C142" s="1">
-        <v>256936</v>
+        <v>130643.3671875</v>
       </c>
       <c r="D142" s="2">
         <v>4579196</v>
       </c>
       <c r="E142" s="1">
-        <v>1.549502748332543e-08</v>
+        <v>7.8787039115013613e-09</v>
       </c>
     </row>
     <row r="143">
@@ -2527,13 +2527,13 @@
         <v>7</v>
       </c>
       <c r="C143" s="1">
-        <v>155265.953125</v>
+        <v>78947.546875</v>
       </c>
       <c r="D143" s="2">
         <v>4579196</v>
       </c>
       <c r="E143" s="1">
-        <v>1.7490538795073007e-08</v>
+        <v>8.8933544972746859e-09</v>
       </c>
     </row>
     <row r="144">
@@ -2544,13 +2544,13 @@
         <v>7</v>
       </c>
       <c r="C144" s="1">
-        <v>104586.5625</v>
+        <v>53178.76953125</v>
       </c>
       <c r="D144" s="2">
         <v>4579196</v>
       </c>
       <c r="E144" s="1">
-        <v>8.4219884399772127e-09</v>
+        <v>4.2822994039681817e-09</v>
       </c>
     </row>
     <row r="145">
@@ -2561,13 +2561,13 @@
         <v>7</v>
       </c>
       <c r="C145" s="1">
-        <v>35994.23046875</v>
+        <v>18301.86328125</v>
       </c>
       <c r="D145" s="2">
         <v>4579196</v>
       </c>
       <c r="E145" s="1">
-        <v>4.0809164936206344e-09</v>
+        <v>2.0750097196042816e-09</v>
       </c>
     </row>
     <row r="146">
@@ -2578,13 +2578,13 @@
         <v>7</v>
       </c>
       <c r="C146" s="1">
-        <v>65355.14453125</v>
+        <v>33230.90625</v>
       </c>
       <c r="D146" s="2">
         <v>4579196</v>
       </c>
       <c r="E146" s="1">
-        <v>7.1919137312193016e-09</v>
+        <v>3.6568477135290323e-09</v>
       </c>
     </row>
     <row r="147">
@@ -2595,13 +2595,13 @@
         <v>7</v>
       </c>
       <c r="C147" s="1">
-        <v>56715.99609375</v>
+        <v>28838.1875</v>
       </c>
       <c r="D147" s="2">
         <v>4579196</v>
       </c>
       <c r="E147" s="1">
-        <v>1.3677985855053976e-08</v>
+        <v>6.9547985148687985e-09</v>
       </c>
     </row>
     <row r="148">
@@ -2612,13 +2612,13 @@
         <v>7</v>
       </c>
       <c r="C148" s="1">
-        <v>11562.5751953125</v>
+        <v>5879.18310546875</v>
       </c>
       <c r="D148" s="2">
         <v>4579196</v>
       </c>
       <c r="E148" s="1">
-        <v>2.7625388643315318e-09</v>
+        <v>1.404658722670149e-09</v>
       </c>
     </row>
     <row r="149">
@@ -2629,13 +2629,13 @@
         <v>7</v>
       </c>
       <c r="C149" s="1">
-        <v>618.46783447265625</v>
+        <v>314.47021484375</v>
       </c>
       <c r="D149" s="2">
         <v>4579196</v>
       </c>
       <c r="E149" s="1">
-        <v>3.2176694642060966e-10</v>
+        <v>1.6360772459034223e-10</v>
       </c>
     </row>
     <row r="150">
@@ -2663,13 +2663,13 @@
         <v>7</v>
       </c>
       <c r="C151" s="1">
-        <v>3092.11279296875</v>
+        <v>1572.2359619140625</v>
       </c>
       <c r="D151" s="2">
         <v>4579196</v>
       </c>
       <c r="E151" s="1">
-        <v>4.6391375185805828e-09</v>
+        <v>2.3588462294554802e-09</v>
       </c>
     </row>
     <row r="152">
@@ -2680,13 +2680,13 @@
         <v>7</v>
       </c>
       <c r="C152" s="1">
-        <v>3269.809326171875</v>
+        <v>1662.5887451171875</v>
       </c>
       <c r="D152" s="2">
         <v>4579196</v>
       </c>
       <c r="E152" s="1">
-        <v>1.2497414658696471e-08</v>
+        <v>6.3545178008439507e-09</v>
       </c>
     </row>
     <row r="153">
@@ -2697,13 +2697,13 @@
         <v>7</v>
       </c>
       <c r="C153" s="1">
-        <v>3269.809326171875</v>
+        <v>1662.5887451171875</v>
       </c>
       <c r="D153" s="2">
         <v>4579196</v>
       </c>
       <c r="E153" s="1">
-        <v>2.4994831093749781e-08</v>
+        <v>1.2709036489866321e-08</v>
       </c>
     </row>
     <row r="154">
@@ -2714,13 +2714,13 @@
         <v>8</v>
       </c>
       <c r="C154" s="1">
-        <v>4273.994140625</v>
+        <v>4344.2998046875</v>
       </c>
       <c r="D154" s="2">
         <v>3474730</v>
       </c>
       <c r="E154" s="1">
-        <v>9.9057839708649453e-10</v>
+        <v>1.0068730293966155e-09</v>
       </c>
     </row>
     <row r="155">
@@ -2731,13 +2731,13 @@
         <v>8</v>
       </c>
       <c r="C155" s="1">
-        <v>19374.87109375</v>
+        <v>20007.62109375</v>
       </c>
       <c r="D155" s="2">
         <v>3474730</v>
       </c>
       <c r="E155" s="1">
-        <v>3.6584363316549684e-10</v>
+        <v>3.7779146477845416e-10</v>
       </c>
     </row>
     <row r="156">
@@ -2748,13 +2748,13 @@
         <v>8</v>
       </c>
       <c r="C156" s="1">
-        <v>27985.92578125</v>
+        <v>28899.896484375</v>
       </c>
       <c r="D156" s="2">
         <v>3474730</v>
       </c>
       <c r="E156" s="1">
-        <v>4.3902217972124902e-10</v>
+        <v>4.5335984966143883e-10</v>
       </c>
     </row>
     <row r="157">
@@ -2765,13 +2765,13 @@
         <v>8</v>
       </c>
       <c r="C157" s="1">
-        <v>45208.03125</v>
+        <v>46684.4453125</v>
       </c>
       <c r="D157" s="2">
         <v>3474730</v>
       </c>
       <c r="E157" s="1">
-        <v>6.26229568201353e-10</v>
+        <v>6.4668109756027548e-10</v>
       </c>
     </row>
     <row r="158">
@@ -2782,13 +2782,13 @@
         <v>8</v>
       </c>
       <c r="C158" s="1">
-        <v>152846.1875</v>
+        <v>157837.875</v>
       </c>
       <c r="D158" s="2">
         <v>3474730</v>
       </c>
       <c r="E158" s="1">
-        <v>5.4094790868930431e-09</v>
+        <v>5.5861431036419162e-09</v>
       </c>
     </row>
     <row r="159">
@@ -2799,13 +2799,13 @@
         <v>8</v>
       </c>
       <c r="C159" s="1">
-        <v>531977.8125</v>
+        <v>549351.25</v>
       </c>
       <c r="D159" s="2">
         <v>3474730</v>
       </c>
       <c r="E159" s="1">
-        <v>1.9589776911743684e-08</v>
+        <v>2.022954248559472e-08</v>
       </c>
     </row>
     <row r="160">
@@ -2816,13 +2816,13 @@
         <v>8</v>
       </c>
       <c r="C160" s="1">
-        <v>907214.625</v>
+        <v>936842.6875</v>
       </c>
       <c r="D160" s="2">
         <v>3474730</v>
       </c>
       <c r="E160" s="1">
-        <v>4.5133333514968399e-08</v>
+        <v>4.6607311787738581e-08</v>
       </c>
     </row>
     <row r="161">
@@ -2833,13 +2833,13 @@
         <v>8</v>
       </c>
       <c r="C161" s="1">
-        <v>1261708.125</v>
+        <v>1302913.375</v>
       </c>
       <c r="D161" s="2">
         <v>3474730</v>
       </c>
       <c r="E161" s="1">
-        <v>4.6660378671958824e-08</v>
+        <v>4.8184229939352008e-08</v>
       </c>
     </row>
     <row r="162">
@@ -2850,13 +2850,13 @@
         <v>8</v>
       </c>
       <c r="C162" s="1">
-        <v>1520353.25</v>
+        <v>1570005.25</v>
       </c>
       <c r="D162" s="2">
         <v>3474730</v>
       </c>
       <c r="E162" s="1">
-        <v>4.1851990317809395e-08</v>
+        <v>4.3218800982458561e-08</v>
       </c>
     </row>
     <row r="163">
@@ -2867,13 +2867,13 @@
         <v>8</v>
       </c>
       <c r="C163" s="1">
-        <v>1621932.125</v>
+        <v>1674901.5</v>
       </c>
       <c r="D163" s="2">
         <v>3474730</v>
       </c>
       <c r="E163" s="1">
-        <v>2.5708533968327174e-08</v>
+        <v>2.6548127252112863e-08</v>
       </c>
     </row>
     <row r="164">
@@ -2884,13 +2884,13 @@
         <v>8</v>
       </c>
       <c r="C164" s="1">
-        <v>1309142.625</v>
+        <v>1351896.875</v>
       </c>
       <c r="D164" s="2">
         <v>3474730</v>
       </c>
       <c r="E164" s="1">
-        <v>4.2431942404164147e-08</v>
+        <v>4.3817696138148676e-08</v>
       </c>
     </row>
     <row r="165">
@@ -2901,13 +2901,13 @@
         <v>8</v>
       </c>
       <c r="C165" s="1">
-        <v>829804.625</v>
+        <v>856904.5625</v>
       </c>
       <c r="D165" s="2">
         <v>3474730</v>
       </c>
       <c r="E165" s="1">
-        <v>2.9514243493622416e-08</v>
+        <v>3.0478126689104101e-08</v>
       </c>
     </row>
     <row r="166">
@@ -2918,13 +2918,13 @@
         <v>8</v>
       </c>
       <c r="C166" s="1">
-        <v>454533.875</v>
+        <v>469480</v>
       </c>
       <c r="D166" s="2">
         <v>3474730</v>
       </c>
       <c r="E166" s="1">
-        <v>2.8344125269086362e-08</v>
+        <v>2.9276145951939725e-08</v>
       </c>
     </row>
     <row r="167">
@@ -2935,13 +2935,13 @@
         <v>8</v>
       </c>
       <c r="C167" s="1">
-        <v>283713.5625</v>
+        <v>165101.734375</v>
       </c>
       <c r="D167" s="2">
         <v>3474730</v>
       </c>
       <c r="E167" s="1">
-        <v>1.8477814833772754e-08</v>
+        <v>1.0752814638692598e-08</v>
       </c>
     </row>
     <row r="168">
@@ -2952,13 +2952,13 @@
         <v>8</v>
       </c>
       <c r="C168" s="1">
-        <v>133172.3125</v>
+        <v>96088.796875</v>
       </c>
       <c r="D168" s="2">
         <v>3474730</v>
       </c>
       <c r="E168" s="1">
-        <v>1.0583992349211258e-08</v>
+        <v>7.6367463464066532e-09</v>
       </c>
     </row>
     <row r="169">
@@ -2969,13 +2969,13 @@
         <v>8</v>
       </c>
       <c r="C169" s="1">
-        <v>138650.78125</v>
+        <v>100041.7109375</v>
       </c>
       <c r="D169" s="2">
         <v>3474730</v>
       </c>
       <c r="E169" s="1">
-        <v>2.0583415860642162e-08</v>
+        <v>1.4851702978546655e-08</v>
       </c>
     </row>
     <row r="170">
@@ -2986,13 +2986,13 @@
         <v>8</v>
       </c>
       <c r="C170" s="1">
-        <v>104533.8359375</v>
+        <v>75425.0625</v>
       </c>
       <c r="D170" s="2">
         <v>3474730</v>
       </c>
       <c r="E170" s="1">
-        <v>1.1093377771942414e-08</v>
+        <v>8.0042861227980211e-09</v>
       </c>
     </row>
     <row r="171">
@@ -3003,13 +3003,13 @@
         <v>8</v>
       </c>
       <c r="C171" s="1">
-        <v>75327.6328125</v>
+        <v>54351.703125</v>
       </c>
       <c r="D171" s="2">
         <v>3474730</v>
       </c>
       <c r="E171" s="1">
-        <v>1.125504667243149e-08</v>
+        <v>8.1209368119061764e-09</v>
       </c>
     </row>
     <row r="172">
@@ -3020,13 +3020,13 @@
         <v>8</v>
       </c>
       <c r="C172" s="1">
-        <v>42512.8984375</v>
+        <v>30674.642578125</v>
       </c>
       <c r="D172" s="2">
         <v>3474730</v>
       </c>
       <c r="E172" s="1">
-        <v>6.1652909444376292e-09</v>
+        <v>4.4484873562566918e-09</v>
       </c>
     </row>
     <row r="173">
@@ -3037,13 +3037,13 @@
         <v>8</v>
       </c>
       <c r="C173" s="1">
-        <v>39996.0078125</v>
+        <v>28858.61328125</v>
       </c>
       <c r="D173" s="2">
         <v>3474730</v>
       </c>
       <c r="E173" s="1">
-        <v>1.2711634411743944e-08</v>
+        <v>9.1719192241157543e-09</v>
       </c>
     </row>
     <row r="174">
@@ -3054,13 +3054,13 @@
         <v>8</v>
       </c>
       <c r="C174" s="1">
-        <v>27883.7890625</v>
+        <v>20119.1953125</v>
       </c>
       <c r="D174" s="2">
         <v>3474730</v>
       </c>
       <c r="E174" s="1">
-        <v>8.7795806180679392e-09</v>
+        <v>6.3347953549452996e-09</v>
       </c>
     </row>
     <row r="175">
@@ -3071,13 +3071,13 @@
         <v>8</v>
       </c>
       <c r="C175" s="1">
-        <v>14032.7177734375</v>
+        <v>10125.1298828125</v>
       </c>
       <c r="D175" s="2">
         <v>3474730</v>
       </c>
       <c r="E175" s="1">
-        <v>9.6213108591314267e-09</v>
+        <v>6.942135311049924e-09</v>
       </c>
     </row>
     <row r="176">
@@ -3088,13 +3088,13 @@
         <v>8</v>
       </c>
       <c r="C176" s="1">
-        <v>7245.53369140625</v>
+        <v>5227.9228515625</v>
       </c>
       <c r="D176" s="2">
         <v>3474730</v>
       </c>
       <c r="E176" s="1">
-        <v>4.9064503571116802e-09</v>
+        <v>3.5401868103690504e-09</v>
       </c>
     </row>
     <row r="177">
@@ -3105,13 +3105,13 @@
         <v>8</v>
       </c>
       <c r="C177" s="1">
-        <v>2425.11083984375</v>
+        <v>1749.8079833984375</v>
       </c>
       <c r="D177" s="2">
         <v>3474730</v>
       </c>
       <c r="E177" s="1">
-        <v>4.7949235693067749e-09</v>
+        <v>3.4597162912319845e-09</v>
       </c>
     </row>
     <row r="178">
@@ -3122,13 +3122,13 @@
         <v>8</v>
       </c>
       <c r="C178" s="1">
-        <v>5209.29150390625</v>
+        <v>3758.697998046875</v>
       </c>
       <c r="D178" s="2">
         <v>3474730</v>
       </c>
       <c r="E178" s="1">
-        <v>2.6238836881020688e-08</v>
+        <v>1.8932299283846987e-08</v>
       </c>
     </row>
     <row r="179">
@@ -3139,13 +3139,13 @@
         <v>8</v>
       </c>
       <c r="C179" s="1">
-        <v>1914.481201171875</v>
+        <v>1381.36962890625</v>
       </c>
       <c r="D179" s="2">
         <v>3474730</v>
       </c>
       <c r="E179" s="1">
-        <v>1.9286217067815414e-08</v>
+        <v>1.3915725460833528e-08</v>
       </c>
     </row>
     <row r="180">
@@ -3173,13 +3173,13 @@
         <v>9</v>
       </c>
       <c r="C181" s="1">
-        <v>3494.67724609375</v>
+        <v>3634.8701171875</v>
       </c>
       <c r="D181" s="2">
         <v>472523</v>
       </c>
       <c r="E181" s="1">
-        <v>4.0313635762956324e-10</v>
+        <v>4.1930861560679489e-10</v>
       </c>
     </row>
     <row r="182">
@@ -3190,13 +3190,13 @@
         <v>9</v>
       </c>
       <c r="C182" s="1">
-        <v>10484.03125</v>
+        <v>10904.6103515625</v>
       </c>
       <c r="D182" s="2">
         <v>472523</v>
       </c>
       <c r="E182" s="1">
-        <v>1.0679339634833696e-09</v>
+        <v>1.1107753605799076e-09</v>
       </c>
     </row>
     <row r="183">
@@ -3207,13 +3207,13 @@
         <v>9</v>
       </c>
       <c r="C183" s="1">
-        <v>9319.1396484375</v>
+        <v>9692.9873046875</v>
       </c>
       <c r="D183" s="2">
         <v>472523</v>
       </c>
       <c r="E183" s="1">
-        <v>2.4253519192996009e-09</v>
+        <v>2.5226476463302561e-09</v>
       </c>
     </row>
     <row r="184">
@@ -3224,13 +3224,13 @@
         <v>9</v>
       </c>
       <c r="C184" s="1">
-        <v>32616.98828125</v>
+        <v>33925.453125</v>
       </c>
       <c r="D184" s="2">
         <v>472523</v>
       </c>
       <c r="E184" s="1">
-        <v>8.8323837132975314e-09</v>
+        <v>9.1867038420900826e-09</v>
       </c>
     </row>
     <row r="185">
@@ -3241,13 +3241,13 @@
         <v>9</v>
       </c>
       <c r="C185" s="1">
-        <v>96520.953125</v>
+        <v>100393</v>
       </c>
       <c r="D185" s="2">
         <v>472523</v>
       </c>
       <c r="E185" s="1">
-        <v>3.5310762314111344e-08</v>
+        <v>3.6727293206695322e-08</v>
       </c>
     </row>
     <row r="186">
@@ -3258,13 +3258,13 @@
         <v>9</v>
       </c>
       <c r="C186" s="1">
-        <v>129319.34375</v>
+        <v>134507.125</v>
       </c>
       <c r="D186" s="2">
         <v>472523</v>
       </c>
       <c r="E186" s="1">
-        <v>3.5168266521168334e-08</v>
+        <v>3.6579081097443122e-08</v>
       </c>
     </row>
     <row r="187">
@@ -3275,13 +3275,13 @@
         <v>9</v>
       </c>
       <c r="C187" s="1">
-        <v>138940.484375</v>
+        <v>144514.234375</v>
       </c>
       <c r="D187" s="2">
         <v>472523</v>
       </c>
       <c r="E187" s="1">
-        <v>2.8125390016953133e-08</v>
+        <v>2.9253669708850794e-08</v>
       </c>
     </row>
     <row r="188">
@@ -3292,13 +3292,13 @@
         <v>9</v>
       </c>
       <c r="C188" s="1">
-        <v>224567.453125</v>
+        <v>233576.234375</v>
       </c>
       <c r="D188" s="2">
         <v>472523</v>
       </c>
       <c r="E188" s="1">
-        <v>2.6175172251896583e-08</v>
+        <v>2.7225219412230217e-08</v>
       </c>
     </row>
     <row r="189">
@@ -3309,13 +3309,13 @@
         <v>9</v>
       </c>
       <c r="C189" s="1">
-        <v>234207.953125</v>
+        <v>243603.46875</v>
       </c>
       <c r="D189" s="2">
         <v>472523</v>
       </c>
       <c r="E189" s="1">
-        <v>5.5822042099862301e-08</v>
+        <v>5.8061406349452227e-08</v>
       </c>
     </row>
     <row r="190">
@@ -3326,13 +3326,13 @@
         <v>9</v>
       </c>
       <c r="C190" s="1">
-        <v>244838.5</v>
+        <v>254660.453125</v>
       </c>
       <c r="D190" s="2">
         <v>472523</v>
       </c>
       <c r="E190" s="1">
-        <v>6.403739405413944e-08</v>
+        <v>6.6606318682715937e-08</v>
       </c>
     </row>
     <row r="191">
@@ -3343,13 +3343,13 @@
         <v>9</v>
       </c>
       <c r="C191" s="1">
-        <v>103382.1171875</v>
+        <v>107529.3984375</v>
       </c>
       <c r="D191" s="2">
         <v>472523</v>
       </c>
       <c r="E191" s="1">
-        <v>4.7406768288738022e-08</v>
+        <v>4.9308539473713608e-08</v>
       </c>
     </row>
     <row r="192">
@@ -3360,13 +3360,13 @@
         <v>9</v>
       </c>
       <c r="C192" s="1">
-        <v>49250.203125</v>
+        <v>58113.5859375</v>
       </c>
       <c r="D192" s="2">
         <v>472523</v>
       </c>
       <c r="E192" s="1">
-        <v>2.3587213959785913e-08</v>
+        <v>2.783212060819551e-08</v>
       </c>
     </row>
     <row r="193">
@@ -3377,13 +3377,13 @@
         <v>9</v>
       </c>
       <c r="C193" s="1">
-        <v>87619.96875</v>
+        <v>67729.8125</v>
       </c>
       <c r="D193" s="2">
         <v>472523</v>
       </c>
       <c r="E193" s="1">
-        <v>5.1207880602532896e-08</v>
+        <v>3.9583444078061802e-08</v>
       </c>
     </row>
     <row r="194">
@@ -3394,13 +3394,13 @@
         <v>9</v>
       </c>
       <c r="C194" s="1">
-        <v>76262.859375</v>
+        <v>58950.8203125</v>
       </c>
       <c r="D194" s="2">
         <v>472523</v>
       </c>
       <c r="E194" s="1">
-        <v>8.3254235505592078e-08</v>
+        <v>6.4355120343861927e-08</v>
       </c>
     </row>
     <row r="195">
@@ -3411,13 +3411,13 @@
         <v>9</v>
       </c>
       <c r="C195" s="1">
-        <v>22555.12109375</v>
+        <v>17435</v>
       </c>
       <c r="D195" s="2">
         <v>472523</v>
       </c>
       <c r="E195" s="1">
-        <v>1.7601520241328217e-08</v>
+        <v>1.3605890636370077e-08</v>
       </c>
     </row>
     <row r="196">
@@ -3428,13 +3428,13 @@
         <v>9</v>
       </c>
       <c r="C196" s="1">
-        <v>16857.466796875</v>
+        <v>13030.740234375</v>
       </c>
       <c r="D196" s="2">
         <v>472523</v>
       </c>
       <c r="E196" s="1">
-        <v>1.8521808087257341e-08</v>
+        <v>1.4317268259844695e-08</v>
       </c>
     </row>
     <row r="197">
@@ -3445,13 +3445,13 @@
         <v>9</v>
       </c>
       <c r="C197" s="1">
-        <v>22861.814453125</v>
+        <v>17672.072265625</v>
       </c>
       <c r="D197" s="2">
         <v>472523</v>
       </c>
       <c r="E197" s="1">
-        <v>2.4380447882776934e-08</v>
+        <v>1.8845968341452135e-08</v>
       </c>
     </row>
     <row r="198">
@@ -3462,13 +3462,13 @@
         <v>9</v>
       </c>
       <c r="C198" s="1">
-        <v>3965.51611328125</v>
+        <v>3065.32470703125</v>
       </c>
       <c r="D198" s="2">
         <v>472523</v>
       </c>
       <c r="E198" s="1">
-        <v>9.2679268703932394e-09</v>
+        <v>7.164062232334345e-09</v>
       </c>
     </row>
     <row r="199">
@@ -3479,13 +3479,13 @@
         <v>9</v>
       </c>
       <c r="C199" s="1">
-        <v>5354.44775390625</v>
+        <v>4138.96240234375</v>
       </c>
       <c r="D199" s="2">
         <v>472523</v>
       </c>
       <c r="E199" s="1">
-        <v>1.2397519455475958e-08</v>
+        <v>9.5832231039594262e-09</v>
       </c>
     </row>
     <row r="200">
@@ -3496,13 +3496,13 @@
         <v>9</v>
       </c>
       <c r="C200" s="1">
-        <v>14409.822265625</v>
+        <v>11138.72265625</v>
       </c>
       <c r="D200" s="2">
         <v>472523</v>
       </c>
       <c r="E200" s="1">
-        <v>7.2652269977879769e-08</v>
+        <v>5.6159855432724726e-08</v>
       </c>
     </row>
     <row r="201">
@@ -3513,13 +3513,13 @@
         <v>9</v>
       </c>
       <c r="C201" s="1">
-        <v>743.8675537109375</v>
+        <v>575.0059814453125</v>
       </c>
       <c r="D201" s="2">
         <v>472523</v>
       </c>
       <c r="E201" s="1">
-        <v>3.7041685274630254e-09</v>
+        <v>2.8633042603587455e-09</v>
       </c>
     </row>
     <row r="202">
@@ -3530,13 +3530,13 @@
         <v>9</v>
       </c>
       <c r="C202" s="1">
-        <v>5348.69677734375</v>
+        <v>4134.5166015625</v>
       </c>
       <c r="D202" s="2">
         <v>472523</v>
       </c>
       <c r="E202" s="1">
-        <v>7.7767147388385638e-08</v>
+        <v>6.0113627853297658e-08</v>
       </c>
     </row>
     <row r="203">
@@ -3547,13 +3547,13 @@
         <v>9</v>
       </c>
       <c r="C203" s="1">
-        <v>21.963224411010742</v>
+        <v>16.977466583251953</v>
       </c>
       <c r="D203" s="2">
         <v>472523</v>
       </c>
       <c r="E203" s="1">
-        <v>8.135048190638372e-10</v>
+        <v>6.2883531715129948e-10</v>
       </c>
     </row>
     <row r="204">
@@ -3581,13 +3581,13 @@
         <v>10</v>
       </c>
       <c r="C205" s="1">
-        <v>42157.80029296875</v>
+        <v>43574.60791015625</v>
       </c>
       <c r="D205" s="2">
         <v>785624</v>
       </c>
       <c r="E205" s="1">
-        <v>4.3215464984314167e-08</v>
+        <v>4.4667817888921491e-08</v>
       </c>
     </row>
     <row r="206">
@@ -3598,13 +3598,13 @@
         <v>10</v>
       </c>
       <c r="C206" s="1">
-        <v>72246.0390625</v>
+        <v>74942.4140625</v>
       </c>
       <c r="D206" s="2">
         <v>785624</v>
       </c>
       <c r="E206" s="1">
-        <v>6.0336073914868393e-09</v>
+        <v>6.2587943716607697e-09</v>
       </c>
     </row>
     <row r="207">
@@ -3615,13 +3615,13 @@
         <v>10</v>
       </c>
       <c r="C207" s="1">
-        <v>79990.453125</v>
+        <v>82975.8671875</v>
       </c>
       <c r="D207" s="2">
         <v>785624</v>
       </c>
       <c r="E207" s="1">
-        <v>5.5499778106593567e-09</v>
+        <v>5.7571147848989312e-09</v>
       </c>
     </row>
     <row r="208">
@@ -3632,13 +3632,13 @@
         <v>10</v>
       </c>
       <c r="C208" s="1">
-        <v>103798.0234375</v>
+        <v>107671.9921875</v>
       </c>
       <c r="D208" s="2">
         <v>785624</v>
       </c>
       <c r="E208" s="1">
-        <v>6.3593592614097361e-09</v>
+        <v>6.5967045159709414e-09</v>
       </c>
     </row>
     <row r="209">
@@ -3649,13 +3649,13 @@
         <v>10</v>
       </c>
       <c r="C209" s="1">
-        <v>185740.53125</v>
+        <v>192672.78125</v>
       </c>
       <c r="D209" s="2">
         <v>785624</v>
       </c>
       <c r="E209" s="1">
-        <v>2.9074605834011891e-08</v>
+        <v>3.0159736041923679e-08</v>
       </c>
     </row>
     <row r="210">
@@ -3666,13 +3666,13 @@
         <v>10</v>
       </c>
       <c r="C210" s="1">
-        <v>322673.34375</v>
+        <v>334716.21875</v>
       </c>
       <c r="D210" s="2">
         <v>785624</v>
       </c>
       <c r="E210" s="1">
-        <v>5.2553950524725224e-08</v>
+        <v>5.4515378877795229e-08</v>
       </c>
     </row>
     <row r="211">
@@ -3683,13 +3683,13 @@
         <v>10</v>
       </c>
       <c r="C211" s="1">
-        <v>203484.234375</v>
+        <v>211078.703125</v>
       </c>
       <c r="D211" s="2">
         <v>785624</v>
       </c>
       <c r="E211" s="1">
-        <v>4.477385218137897e-08</v>
+        <v>4.6444910140053253e-08</v>
       </c>
     </row>
     <row r="212">
@@ -3700,13 +3700,13 @@
         <v>10</v>
       </c>
       <c r="C212" s="1">
-        <v>109995.8203125</v>
+        <v>114101.1015625</v>
       </c>
       <c r="D212" s="2">
         <v>785624</v>
       </c>
       <c r="E212" s="1">
-        <v>1.7991686362961445e-08</v>
+        <v>1.8663175893607331e-08</v>
       </c>
     </row>
     <row r="213">
@@ -3717,13 +3717,13 @@
         <v>10</v>
       </c>
       <c r="C213" s="1">
-        <v>89069.2734375</v>
+        <v>92393.53125</v>
       </c>
       <c r="D213" s="2">
         <v>785624</v>
       </c>
       <c r="E213" s="1">
-        <v>1.0844408038224174e-08</v>
+        <v>1.1249144726832583e-08</v>
       </c>
     </row>
     <row r="214">
@@ -3734,13 +3734,13 @@
         <v>10</v>
       </c>
       <c r="C214" s="1">
-        <v>94129.8828125</v>
+        <v>97665.8984375</v>
       </c>
       <c r="D214" s="2">
         <v>785624</v>
       </c>
       <c r="E214" s="1">
-        <v>6.5990053421671746e-09</v>
+        <v>6.8468986036407387e-09</v>
       </c>
     </row>
     <row r="215">
@@ -3751,13 +3751,13 @@
         <v>10</v>
       </c>
       <c r="C215" s="1">
-        <v>48507.75</v>
+        <v>48047.7734375</v>
       </c>
       <c r="D215" s="2">
         <v>785624</v>
       </c>
       <c r="E215" s="1">
-        <v>6.9538192981610791e-09</v>
+        <v>6.8878796000149123e-09</v>
       </c>
     </row>
     <row r="216">
@@ -3768,13 +3768,13 @@
         <v>10</v>
       </c>
       <c r="C216" s="1">
-        <v>68175.4453125</v>
+        <v>48367.375</v>
       </c>
       <c r="D216" s="2">
         <v>785624</v>
       </c>
       <c r="E216" s="1">
-        <v>1.0724822807617329e-08</v>
+        <v>7.6087731670781977e-09</v>
       </c>
     </row>
     <row r="217">
@@ -3785,13 +3785,13 @@
         <v>10</v>
       </c>
       <c r="C217" s="1">
-        <v>35136.44140625</v>
+        <v>24927.705078125</v>
       </c>
       <c r="D217" s="2">
         <v>785624</v>
       </c>
       <c r="E217" s="1">
-        <v>9.6908285840413555e-09</v>
+        <v>6.8752012971629028e-09</v>
       </c>
     </row>
     <row r="218">
@@ -3802,13 +3802,13 @@
         <v>10</v>
       </c>
       <c r="C218" s="1">
-        <v>35360.6796875</v>
+        <v>25086.791015625</v>
       </c>
       <c r="D218" s="2">
         <v>785624</v>
       </c>
       <c r="E218" s="1">
-        <v>1.0185853938082801e-08</v>
+        <v>7.2263990347209983e-09</v>
       </c>
     </row>
     <row r="219">
@@ -3819,13 +3819,13 @@
         <v>10</v>
       </c>
       <c r="C219" s="1">
-        <v>18247.61328125</v>
+        <v>12945.849609375</v>
       </c>
       <c r="D219" s="2">
         <v>785624</v>
       </c>
       <c r="E219" s="1">
-        <v>6.4142811062595229e-09</v>
+        <v>4.5506398649308721e-09</v>
       </c>
     </row>
     <row r="220">
@@ -3836,13 +3836,13 @@
         <v>10</v>
       </c>
       <c r="C220" s="1">
-        <v>3944.017822265625</v>
+        <v>2798.10107421875</v>
       </c>
       <c r="D220" s="2">
         <v>785624</v>
       </c>
       <c r="E220" s="1">
-        <v>2.5896456090634956e-09</v>
+        <v>1.8372355858886635e-09</v>
       </c>
     </row>
     <row r="221">
@@ -3853,13 +3853,13 @@
         <v>10</v>
       </c>
       <c r="C221" s="1">
-        <v>2822.2900390625</v>
+        <v>2002.2862548828125</v>
       </c>
       <c r="D221" s="2">
         <v>785624</v>
       </c>
       <c r="E221" s="1">
-        <v>1.3246919117193556e-09</v>
+        <v>9.398085643042009e-10</v>
       </c>
     </row>
     <row r="222">
@@ -3870,13 +3870,13 @@
         <v>10</v>
       </c>
       <c r="C222" s="1">
-        <v>511.51873779296875</v>
+        <v>362.89923095703125</v>
       </c>
       <c r="D222" s="2">
         <v>785624</v>
       </c>
       <c r="E222" s="1">
-        <v>3.3803435051105168e-10</v>
+        <v>2.3981996943867046e-10</v>
       </c>
     </row>
     <row r="223">
@@ -3904,13 +3904,13 @@
         <v>10</v>
       </c>
       <c r="C224" s="1">
-        <v>3.2261433601379395</v>
+        <v>2.288801908493042</v>
       </c>
       <c r="D224" s="2">
         <v>785624</v>
       </c>
       <c r="E224" s="1">
-        <v>4.5349735251776213e-12</v>
+        <v>3.2173571532650991e-12</v>
       </c>
     </row>
     <row r="225">
@@ -3921,13 +3921,13 @@
         <v>10</v>
       </c>
       <c r="C225" s="1">
-        <v>1169.64208984375</v>
+        <v>829.80780029296875</v>
       </c>
       <c r="D225" s="2">
         <v>785624</v>
       </c>
       <c r="E225" s="1">
-        <v>1.6288508319917128e-09</v>
+        <v>1.155595508173235e-09</v>
       </c>
     </row>
     <row r="226">

</xml_diff>

<commit_message>
updated and new files
The updated recreational selectivity file calculates rec selectivity based on the proportion of biomass available in the baseline year, rather than assuming all states have equal availability. The state biomass proportion files gives the projected biomass proportions under no shift (year=2019) or under a shift scenario (year 2020+). In the "catch at length given stock structure - prediction.R", we must first multiply total numbers at length by the state proportion of biomass. Then, new numbers-at-length by state is used to calculate the catch adjustment factor.
</commit_message>
<xml_diff>
--- a/rec_selectivity_by_state_cdf_star_raw_18_19.xlsx
+++ b/rec_selectivity_by_state_cdf_star_raw_18_19.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="14">
   <si>
     <t>l_in_bin</t>
   </si>
@@ -102,7 +102,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E230"/>
+  <dimension ref="A1:E235"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -124,3895 +124,3980 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2">
         <v>413071</v>
       </c>
       <c r="E2" s="1">
-        <v>0</v>
+        <v>1.1609237009213569e-11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>7382.95458984375</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2">
         <v>413071</v>
       </c>
       <c r="E3" s="1">
-        <v>9.7425656431227026e-10</v>
+        <v>9.4581330614684767e-13</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>9492.3701171875</v>
+        <v>7382.95458984375</v>
       </c>
       <c r="D4" s="2">
         <v>413071</v>
       </c>
       <c r="E4" s="1">
-        <v>1.1060862226131007e-09</v>
+        <v>5.8013052139926913e-09</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1">
-        <v>21094.158203125</v>
+        <v>9492.3701171875</v>
       </c>
       <c r="D5" s="2">
         <v>413071</v>
       </c>
       <c r="E5" s="1">
-        <v>6.2799960787174314e-09</v>
+        <v>6.5862977294273151e-09</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="1">
-        <v>15820.6162109375</v>
+        <v>21094.158203125</v>
       </c>
       <c r="D6" s="2">
         <v>413071</v>
       </c>
       <c r="E6" s="1">
-        <v>4.9006727564915309e-09</v>
+        <v>3.7394848106941936e-08</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="1">
-        <v>52735.390625</v>
+        <v>15820.6162109375</v>
       </c>
       <c r="D7" s="2">
         <v>413071</v>
       </c>
       <c r="E7" s="1">
-        <v>2.206916605018705e-08</v>
+        <v>2.9181531857602749e-08</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="1">
-        <v>132927.171875</v>
+        <v>52735.390625</v>
       </c>
       <c r="D8" s="2">
         <v>413071</v>
       </c>
       <c r="E8" s="1">
-        <v>4.1352283375317711e-08</v>
+        <v>1.3141298893515341e-07</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="1">
-        <v>137798.328125</v>
+        <v>132927.171875</v>
       </c>
       <c r="D9" s="2">
         <v>413071</v>
       </c>
       <c r="E9" s="1">
-        <v>3.1908907516253748e-08</v>
+        <v>2.4623619765407057e-07</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="1">
-        <v>136921.75</v>
+        <v>137798.328125</v>
       </c>
       <c r="D10" s="2">
         <v>413071</v>
       </c>
       <c r="E10" s="1">
-        <v>1.8256328004895295e-08</v>
+        <v>1.9000468398644443e-07</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="1">
-        <v>190174.25</v>
+        <v>136921.75</v>
       </c>
       <c r="D11" s="2">
         <v>413071</v>
       </c>
       <c r="E11" s="1">
-        <v>5.1850630455874125e-08</v>
+        <v>1.0870907374282979e-07</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="1">
-        <v>197436.4375</v>
+        <v>190174.25</v>
       </c>
       <c r="D12" s="2">
         <v>413071</v>
       </c>
       <c r="E12" s="1">
-        <v>5.9071702196433762e-08</v>
+        <v>3.0874960543769703e-07</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="1">
-        <v>161044.625</v>
+        <v>197436.4375</v>
       </c>
       <c r="D13" s="2">
         <v>413071</v>
       </c>
       <c r="E13" s="1">
-        <v>8.4477179029818217e-08</v>
+        <v>3.5174818435734778e-07</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="1">
-        <v>41829.15625</v>
+        <v>161044.625</v>
       </c>
       <c r="D14" s="2">
         <v>413071</v>
       </c>
       <c r="E14" s="1">
-        <v>2.2916378128456927e-08</v>
+        <v>5.0302753606956685e-07</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="1">
-        <v>17886.884765625</v>
+        <v>41829.15625</v>
       </c>
       <c r="D15" s="2">
         <v>413071</v>
       </c>
       <c r="E15" s="1">
-        <v>1.1958222856378597e-08</v>
+        <v>1.3645779972648597e-07</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="1">
-        <v>14599.7353515625</v>
+        <v>17886.884765625</v>
       </c>
       <c r="D16" s="2">
         <v>413071</v>
       </c>
       <c r="E16" s="1">
-        <v>1.8232091392178518e-08</v>
+        <v>7.1206400775736256e-08</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="1">
-        <v>8551.65234375</v>
+        <v>14599.7353515625</v>
       </c>
       <c r="D17" s="2">
         <v>413071</v>
       </c>
       <c r="E17" s="1">
-        <v>7.6340205268365935e-09</v>
+        <v>1.0856475540776955e-07</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
       </c>
       <c r="C18" s="1">
-        <v>4908.30029296875</v>
+        <v>8551.65234375</v>
       </c>
       <c r="D18" s="2">
         <v>413071</v>
       </c>
       <c r="E18" s="1">
-        <v>6.1690808017544896e-09</v>
+        <v>4.5457515085445266e-08</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="1">
-        <v>3174.176025390625</v>
+        <v>4908.30029296875</v>
       </c>
       <c r="D19" s="2">
         <v>413071</v>
       </c>
       <c r="E19" s="1">
-        <v>3.8722216544329058e-09</v>
+        <v>3.6734391528625565e-08</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="1">
-        <v>542.42962646484375</v>
+        <v>3174.176025390625</v>
       </c>
       <c r="D20" s="2">
         <v>413071</v>
       </c>
       <c r="E20" s="1">
-        <v>1.4501887468654218e-09</v>
+        <v>2.3057520337488313e-08</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
         <v>2</v>
       </c>
       <c r="C21" s="1">
-        <v>129.90037536621094</v>
+        <v>542.42962646484375</v>
       </c>
       <c r="D21" s="2">
         <v>413071</v>
       </c>
       <c r="E21" s="1">
-        <v>3.4405570059625745e-10</v>
+        <v>8.635289816538716e-09</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
         <v>2</v>
       </c>
       <c r="C22" s="1">
-        <v>293.73092651367188</v>
+        <v>129.90037536621094</v>
       </c>
       <c r="D22" s="2">
         <v>413071</v>
       </c>
       <c r="E22" s="1">
-        <v>1.694097861992816e-09</v>
+        <v>2.0487129770430101e-09</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
         <v>2</v>
       </c>
       <c r="C23" s="1">
-        <v>469.26144409179688</v>
+        <v>293.73092651367188</v>
       </c>
       <c r="D23" s="2">
         <v>413071</v>
       </c>
       <c r="E23" s="1">
-        <v>2.6730571089927935e-09</v>
+        <v>1.008767025467705e-08</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
         <v>2</v>
       </c>
       <c r="C24" s="1">
-        <v>0</v>
+        <v>469.26144409179688</v>
       </c>
       <c r="D24" s="2">
         <v>413071</v>
       </c>
       <c r="E24" s="1">
-        <v>0</v>
+        <v>1.5916977957886047e-08</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
         <v>2</v>
       </c>
       <c r="C25" s="1">
-        <v>34.604843139648438</v>
+        <v>1</v>
       </c>
       <c r="D25" s="2">
         <v>413071</v>
       </c>
       <c r="E25" s="1">
-        <v>1.4662201452964041e-09</v>
+        <v>9.9037306133809011e-11</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
         <v>2</v>
       </c>
       <c r="C26" s="1">
-        <v>0</v>
+        <v>34.604843139648438</v>
       </c>
       <c r="D26" s="2">
         <v>413071</v>
       </c>
       <c r="E26" s="1">
-        <v>0</v>
+        <v>8.7307503449096657e-09</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C27" s="1">
-        <v>3940.27587890625</v>
+        <v>1</v>
       </c>
       <c r="D27" s="2">
-        <v>401288</v>
+        <v>413071</v>
       </c>
       <c r="E27" s="1">
-        <v>6.4424077184099815e-10</v>
+        <v>3.7844777311946132e-10</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
       </c>
       <c r="C28" s="1">
-        <v>3979.85302734375</v>
+        <v>1</v>
       </c>
       <c r="D28" s="2">
         <v>401288</v>
       </c>
       <c r="E28" s="1">
-        <v>5.4060328436023042e-10</v>
+        <v>5.5119631081623766e-11</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B29" t="s">
         <v>3</v>
       </c>
       <c r="C29" s="1">
-        <v>5969.779296875</v>
+        <v>3940.27587890625</v>
       </c>
       <c r="D29" s="2">
         <v>401288</v>
       </c>
       <c r="E29" s="1">
-        <v>7.1604633333777201e-10</v>
+        <v>1.7694352649755274e-08</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="1">
-        <v>11939.8681640625</v>
+        <v>3979.85302734375</v>
       </c>
       <c r="D30" s="2">
         <v>401288</v>
       </c>
       <c r="E30" s="1">
-        <v>3.6590239727019025e-09</v>
+        <v>1.4847905127624017e-08</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B31" t="s">
         <v>3</v>
       </c>
       <c r="C31" s="1">
-        <v>23879.921875</v>
+        <v>5969.779296875</v>
       </c>
       <c r="D31" s="2">
         <v>401288</v>
       </c>
       <c r="E31" s="1">
-        <v>7.6143660265870494e-09</v>
+        <v>1.9666524408989972e-08</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B32" t="s">
         <v>3</v>
       </c>
       <c r="C32" s="1">
-        <v>45768.3125</v>
+        <v>11939.8681640625</v>
       </c>
       <c r="D32" s="2">
         <v>401288</v>
       </c>
       <c r="E32" s="1">
-        <v>1.9715924892693693e-08</v>
+        <v>1.0049668475176077e-07</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B33" t="s">
         <v>3</v>
       </c>
       <c r="C33" s="1">
-        <v>77610.2578125</v>
+        <v>23879.921875</v>
       </c>
       <c r="D33" s="2">
         <v>401288</v>
       </c>
       <c r="E33" s="1">
-        <v>2.4852688795817812e-08</v>
+        <v>2.0913186915549886e-07</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
       </c>
       <c r="C34" s="1">
-        <v>117786.9765625</v>
+        <v>45768.3125</v>
       </c>
       <c r="D34" s="2">
         <v>401288</v>
       </c>
       <c r="E34" s="1">
-        <v>2.8075906044477961e-08</v>
+        <v>5.4150649475559476e-07</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B35" t="s">
         <v>3</v>
       </c>
       <c r="C35" s="1">
-        <v>118327.9453125</v>
+        <v>77610.2578125</v>
       </c>
       <c r="D35" s="2">
         <v>401288</v>
       </c>
       <c r="E35" s="1">
-        <v>1.6240404576706169e-08</v>
+        <v>6.8258992769187898e-07</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B36" t="s">
         <v>3</v>
       </c>
       <c r="C36" s="1">
-        <v>56474.09765625</v>
+        <v>117786.9765625</v>
       </c>
       <c r="D36" s="2">
         <v>401288</v>
       </c>
       <c r="E36" s="1">
-        <v>1.5849668244527493e-08</v>
+        <v>7.7111695873099961e-07</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B37" t="s">
         <v>3</v>
       </c>
       <c r="C37" s="1">
-        <v>26512.328125</v>
+        <v>118327.9453125</v>
       </c>
       <c r="D37" s="2">
         <v>401288</v>
       </c>
       <c r="E37" s="1">
-        <v>8.1652329342318808e-09</v>
+        <v>4.4604976778828132e-07</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B38" t="s">
         <v>3</v>
       </c>
       <c r="C38" s="1">
-        <v>19543.951171875</v>
+        <v>56474.09765625</v>
       </c>
       <c r="D38" s="2">
         <v>401288</v>
       </c>
       <c r="E38" s="1">
-        <v>1.0552954066156417e-08</v>
+        <v>4.3531801452445507e-07</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B39" t="s">
         <v>3</v>
       </c>
       <c r="C39" s="1">
-        <v>10862.0146484375</v>
+        <v>26512.328125</v>
       </c>
       <c r="D39" s="2">
         <v>401288</v>
       </c>
       <c r="E39" s="1">
-        <v>6.1255596150999736e-09</v>
+        <v>2.242616687908594e-07</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B40" t="s">
         <v>3</v>
       </c>
       <c r="C40" s="1">
-        <v>3729.3203125</v>
+        <v>19543.951171875</v>
       </c>
       <c r="D40" s="2">
         <v>401288</v>
       </c>
       <c r="E40" s="1">
-        <v>2.5664343983322624e-09</v>
+        <v>2.8984149480493215e-07</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B41" t="s">
         <v>3</v>
       </c>
       <c r="C41" s="1">
-        <v>1345.5067138671875</v>
+        <v>10862.0146484375</v>
       </c>
       <c r="D41" s="2">
         <v>401288</v>
       </c>
       <c r="E41" s="1">
-        <v>1.7296009069411866e-09</v>
+        <v>1.6824115789404459e-07</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B42" t="s">
         <v>3</v>
       </c>
       <c r="C42" s="1">
-        <v>3192.2021484375</v>
+        <v>3729.3203125</v>
       </c>
       <c r="D42" s="2">
         <v>401288</v>
       </c>
       <c r="E42" s="1">
-        <v>2.9333384610197299e-09</v>
+        <v>7.048823391642145e-08</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B43" t="s">
         <v>3</v>
       </c>
       <c r="C43" s="1">
-        <v>25.691064834594727</v>
+        <v>1345.5067138671875</v>
       </c>
       <c r="D43" s="2">
         <v>401288</v>
       </c>
       <c r="E43" s="1">
-        <v>3.3238387736611585e-11</v>
+        <v>4.7504240541229592e-08</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B44" t="s">
         <v>3</v>
       </c>
       <c r="C44" s="1">
-        <v>254.52424621582031</v>
+        <v>3192.2021484375</v>
       </c>
       <c r="D44" s="2">
         <v>401288</v>
       </c>
       <c r="E44" s="1">
-        <v>3.1961480684294941e-10</v>
+        <v>8.056542100121078e-08</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B45" t="s">
         <v>3</v>
       </c>
       <c r="C45" s="1">
-        <v>178.62748718261719</v>
+        <v>25.691064834594727</v>
       </c>
       <c r="D45" s="2">
         <v>401288</v>
       </c>
       <c r="E45" s="1">
-        <v>4.9158421777661943e-10</v>
+        <v>9.1290680570565996e-10</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B46" t="s">
         <v>3</v>
       </c>
       <c r="C46" s="1">
-        <v>881.1624755859375</v>
+        <v>254.52424621582031</v>
       </c>
       <c r="D46" s="2">
         <v>401288</v>
       </c>
       <c r="E46" s="1">
-        <v>2.4023865119460197e-09</v>
+        <v>8.7783602609192712e-09</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B47" t="s">
         <v>3</v>
       </c>
       <c r="C47" s="1">
-        <v>0</v>
+        <v>178.62748718261719</v>
       </c>
       <c r="D47" s="2">
         <v>401288</v>
       </c>
       <c r="E47" s="1">
-        <v>0</v>
+        <v>1.3501574080976297e-08</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B48" t="s">
         <v>3</v>
       </c>
       <c r="C48" s="1">
-        <v>0</v>
+        <v>881.1624755859375</v>
       </c>
       <c r="D48" s="2">
         <v>401288</v>
       </c>
       <c r="E48" s="1">
-        <v>0</v>
+        <v>6.5982590058411006e-08</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B49" t="s">
         <v>3</v>
       </c>
       <c r="C49" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49" s="2">
         <v>401288</v>
       </c>
       <c r="E49" s="1">
-        <v>0</v>
+        <v>1.6305864991572605e-10</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B50" t="s">
         <v>3</v>
       </c>
       <c r="C50" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50" s="2">
         <v>401288</v>
       </c>
       <c r="E50" s="1">
-        <v>0</v>
+        <v>1.6104542699402202e-10</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B51" t="s">
         <v>3</v>
       </c>
       <c r="C51" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51" s="2">
         <v>401288</v>
       </c>
       <c r="E51" s="1">
-        <v>0</v>
+        <v>4.7022036264721123e-10</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B52" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C52" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52" s="2">
-        <v>104251</v>
+        <v>401288</v>
       </c>
       <c r="E52" s="1">
-        <v>0</v>
+        <v>1.1978910086085648e-09</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B53" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C53" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53" s="2">
-        <v>104251</v>
+        <v>401288</v>
       </c>
       <c r="E53" s="1">
-        <v>0</v>
+        <v>1.7968365684239984e-09</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B54" t="s">
         <v>4</v>
       </c>
       <c r="C54" s="1">
-        <v>9238.4013671875</v>
+        <v>1</v>
       </c>
       <c r="D54" s="2">
         <v>104251</v>
       </c>
       <c r="E54" s="1">
-        <v>1.089779111396183e-08</v>
+        <v>4.5998975461980507e-11</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B55" t="s">
         <v>4</v>
       </c>
       <c r="C55" s="1">
-        <v>9238.4013671875</v>
+        <v>1</v>
       </c>
       <c r="D55" s="2">
         <v>104251</v>
       </c>
       <c r="E55" s="1">
-        <v>1.1338970651308955e-08</v>
+        <v>3.7475712637291547e-12</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B56" t="s">
         <v>4</v>
       </c>
       <c r="C56" s="1">
-        <v>18476.802734375</v>
+        <v>1</v>
       </c>
       <c r="D56" s="2">
         <v>104251</v>
       </c>
       <c r="E56" s="1">
-        <v>3.0637622217000171e-08</v>
+        <v>3.1134363750323635e-12</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B57" t="s">
         <v>4</v>
       </c>
       <c r="C57" s="1">
-        <v>37430.94921875</v>
+        <v>1</v>
       </c>
       <c r="D57" s="2">
         <v>104251</v>
       </c>
       <c r="E57" s="1">
-        <v>4.6138243448012872e-08</v>
+        <v>2.7492307475701638e-12</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B58" t="s">
         <v>4</v>
       </c>
       <c r="C58" s="1">
-        <v>27100.591796875</v>
+        <v>9238.4013671875</v>
       </c>
       <c r="D58" s="2">
         <v>104251</v>
       </c>
       <c r="E58" s="1">
-        <v>2.4865158820830402e-08</v>
+        <v>6.4891956697010755e-08</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B59" t="s">
         <v>4</v>
       </c>
       <c r="C59" s="1">
-        <v>28117.837890625</v>
+        <v>9238.4013671875</v>
       </c>
       <c r="D59" s="2">
         <v>104251</v>
       </c>
       <c r="E59" s="1">
-        <v>1.4854819596621383e-08</v>
+        <v>6.7518996615945071e-08</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B60" t="s">
         <v>4</v>
       </c>
       <c r="C60" s="1">
-        <v>97040.53125</v>
+        <v>18476.802734375</v>
       </c>
       <c r="D60" s="2">
         <v>104251</v>
       </c>
       <c r="E60" s="1">
-        <v>1.0483346812861782e-07</v>
+        <v>1.8243468957734876e-07</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B61" t="s">
         <v>4</v>
       </c>
       <c r="C61" s="1">
-        <v>16215.6904296875</v>
+        <v>37430.94921875</v>
       </c>
       <c r="D61" s="2">
         <v>104251</v>
       </c>
       <c r="E61" s="1">
-        <v>1.9223483249675155e-08</v>
+        <v>2.7473464569993666e-07</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B62" t="s">
         <v>4</v>
       </c>
       <c r="C62" s="1">
-        <v>10365.4443359375</v>
+        <v>27100.591796875</v>
       </c>
       <c r="D62" s="2">
         <v>104251</v>
       </c>
       <c r="E62" s="1">
-        <v>2.1543961281622614e-08</v>
+        <v>1.4806199999384262e-07</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B63" t="s">
         <v>4</v>
       </c>
       <c r="C63" s="1">
-        <v>5789.8037109375</v>
+        <v>28117.837890625</v>
       </c>
       <c r="D63" s="2">
         <v>104251</v>
       </c>
       <c r="E63" s="1">
-        <v>1.2568261098522271e-08</v>
+        <v>8.845446330951745e-08</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B64" t="s">
         <v>4</v>
       </c>
       <c r="C64" s="1">
-        <v>10714.201171875</v>
+        <v>97040.53125</v>
       </c>
       <c r="D64" s="2">
         <v>104251</v>
       </c>
       <c r="E64" s="1">
-        <v>2.8381556660406204e-08</v>
+        <v>6.2424106772596133e-07</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B65" t="s">
         <v>4</v>
       </c>
       <c r="C65" s="1">
-        <v>3806.5068359375</v>
+        <v>16215.6904296875</v>
       </c>
       <c r="D65" s="2">
         <v>104251</v>
       </c>
       <c r="E65" s="1">
-        <v>1.8834867887562723e-08</v>
+        <v>1.1446810077586633e-07</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B66" t="s">
         <v>4</v>
       </c>
       <c r="C66" s="1">
-        <v>3239.448974609375</v>
+        <v>10365.4443359375</v>
       </c>
       <c r="D66" s="2">
         <v>104251</v>
       </c>
       <c r="E66" s="1">
-        <v>1.1458265447572558e-08</v>
+        <v>1.282856061379789e-07</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B67" t="s">
         <v>4</v>
       </c>
       <c r="C67" s="1">
-        <v>2481.369873046875</v>
+        <v>5789.8037109375</v>
       </c>
       <c r="D67" s="2">
         <v>104251</v>
       </c>
       <c r="E67" s="1">
-        <v>1.2357348921909761e-08</v>
+        <v>7.4838929720044689e-08</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B68" t="s">
         <v>4</v>
       </c>
       <c r="C68" s="1">
-        <v>497.12643432617188</v>
+        <v>10714.201171875</v>
       </c>
       <c r="D68" s="2">
         <v>104251</v>
       </c>
       <c r="E68" s="1">
-        <v>2.4029267464698023e-09</v>
+        <v>1.6900074228942685e-07</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B69" t="s">
         <v>4</v>
       </c>
       <c r="C69" s="1">
-        <v>0</v>
+        <v>3806.5068359375</v>
       </c>
       <c r="D69" s="2">
         <v>104251</v>
       </c>
       <c r="E69" s="1">
-        <v>0</v>
+        <v>1.1215405493203434e-07</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B70" t="s">
         <v>4</v>
       </c>
       <c r="C70" s="1">
-        <v>0</v>
+        <v>3239.448974609375</v>
       </c>
       <c r="D70" s="2">
         <v>104251</v>
       </c>
       <c r="E70" s="1">
-        <v>0</v>
+        <v>6.8229354610593873e-08</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B71" t="s">
         <v>4</v>
       </c>
       <c r="C71" s="1">
-        <v>53.702713012695313</v>
+        <v>2481.369873046875</v>
       </c>
       <c r="D71" s="2">
         <v>104251</v>
       </c>
       <c r="E71" s="1">
-        <v>1.2272400873314382e-09</v>
+        <v>7.3583031223733997e-08</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B72" t="s">
         <v>4</v>
       </c>
       <c r="C72" s="1">
-        <v>0</v>
+        <v>497.12643432617188</v>
       </c>
       <c r="D72" s="2">
         <v>104251</v>
       </c>
       <c r="E72" s="1">
-        <v>0</v>
+        <v>1.4308461082634949e-08</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B73" t="s">
         <v>4</v>
       </c>
       <c r="C73" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D73" s="2">
         <v>104251</v>
       </c>
       <c r="E73" s="1">
-        <v>0</v>
+        <v>6.3078008094574756e-11</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B74" t="s">
         <v>4</v>
       </c>
       <c r="C74" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D74" s="2">
         <v>104251</v>
       </c>
       <c r="E74" s="1">
-        <v>0</v>
+        <v>6.2490672358972432e-11</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B75" t="s">
         <v>4</v>
       </c>
       <c r="C75" s="1">
-        <v>0</v>
+        <v>53.702713012695313</v>
       </c>
       <c r="D75" s="2">
         <v>104251</v>
       </c>
       <c r="E75" s="1">
-        <v>0</v>
+        <v>7.3077202067395319e-09</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B76" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C76" s="1">
-        <v>29103.9921875</v>
+        <v>1</v>
       </c>
       <c r="D76" s="2">
-        <v>544681</v>
+        <v>104251</v>
       </c>
       <c r="E76" s="1">
-        <v>4.3031484153743804e-08</v>
+        <v>1.3439720170094205e-10</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B77" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C77" s="1">
-        <v>50032.640625</v>
+        <v>1</v>
       </c>
       <c r="D77" s="2">
-        <v>544681</v>
+        <v>104251</v>
       </c>
       <c r="E77" s="1">
-        <v>6.0268301460553175e-09</v>
+        <v>3.9241293547931377e-10</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B78" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C78" s="1">
-        <v>55395.890625</v>
+        <v>1</v>
       </c>
       <c r="D78" s="2">
-        <v>544681</v>
+        <v>104251</v>
       </c>
       <c r="E78" s="1">
-        <v>5.5437436863314815e-09</v>
+        <v>9.9967567557257553e-10</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B79" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C79" s="1">
-        <v>71883.3828125</v>
+        <v>1</v>
       </c>
       <c r="D79" s="2">
-        <v>544681</v>
+        <v>104251</v>
       </c>
       <c r="E79" s="1">
-        <v>6.3522169746477175e-09</v>
+        <v>1.4995137354034682e-09</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B80" t="s">
         <v>5</v>
       </c>
       <c r="C80" s="1">
-        <v>128631.1328125</v>
+        <v>29103.9921875</v>
       </c>
       <c r="D80" s="2">
         <v>544681</v>
       </c>
       <c r="E80" s="1">
-        <v>2.9041949289876356e-08</v>
+        <v>1.1818784741990385e-06</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B81" t="s">
         <v>5</v>
       </c>
       <c r="C81" s="1">
-        <v>223461.390625</v>
+        <v>50032.640625</v>
       </c>
       <c r="D81" s="2">
         <v>544681</v>
       </c>
       <c r="E81" s="1">
-        <v>5.2494922186951953e-08</v>
+        <v>1.6552951365156332e-07</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B82" t="s">
         <v>5</v>
       </c>
       <c r="C82" s="1">
-        <v>140919.203125</v>
+        <v>55395.890625</v>
       </c>
       <c r="D82" s="2">
         <v>544681</v>
       </c>
       <c r="E82" s="1">
-        <v>4.4723563519255549e-08</v>
+        <v>1.5226133598389424e-07</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B83" t="s">
         <v>5</v>
       </c>
       <c r="C83" s="1">
-        <v>76175.546875</v>
+        <v>71883.3828125</v>
       </c>
       <c r="D83" s="2">
         <v>544681</v>
       </c>
       <c r="E83" s="1">
-        <v>1.7971478527556428e-08</v>
+        <v>1.7446639333229541e-07</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B84" t="s">
         <v>5</v>
       </c>
       <c r="C84" s="1">
-        <v>61683.2578125</v>
+        <v>128631.1328125</v>
       </c>
       <c r="D84" s="2">
         <v>544681</v>
       </c>
       <c r="E84" s="1">
-        <v>1.0832227559376406e-08</v>
+        <v>7.9764976135265897e-07</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B85" t="s">
         <v>5</v>
       </c>
       <c r="C85" s="1">
-        <v>65187.88671875</v>
+        <v>223461.390625</v>
       </c>
       <c r="D85" s="2">
         <v>544681</v>
       </c>
       <c r="E85" s="1">
-        <v>6.5915926050763574e-09</v>
+        <v>1.4417958027479472e-06</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B86" t="s">
         <v>5</v>
       </c>
       <c r="C86" s="1">
-        <v>33684.73828125</v>
+        <v>140919.203125</v>
       </c>
       <c r="D86" s="2">
         <v>544681</v>
       </c>
       <c r="E86" s="1">
-        <v>6.9649495060275513e-09</v>
+        <v>1.228352061843907e-06</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B87" t="s">
         <v>5</v>
       </c>
       <c r="C87" s="1">
-        <v>33559.91015625</v>
+        <v>76175.546875</v>
       </c>
       <c r="D87" s="2">
         <v>544681</v>
       </c>
       <c r="E87" s="1">
-        <v>7.6147461669506811e-09</v>
+        <v>4.9359442755303462e-07</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B88" t="s">
         <v>5</v>
       </c>
       <c r="C88" s="1">
-        <v>17296.1953125</v>
+        <v>61683.2578125</v>
       </c>
       <c r="D88" s="2">
         <v>544681</v>
       </c>
       <c r="E88" s="1">
-        <v>6.8805987574194205e-09</v>
+        <v>2.9751183205917187e-07</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B89" t="s">
         <v>5</v>
       </c>
       <c r="C89" s="1">
-        <v>17406.576171875</v>
+        <v>65187.88671875</v>
       </c>
       <c r="D89" s="2">
         <v>544681</v>
       </c>
       <c r="E89" s="1">
-        <v>7.2320713861984132e-09</v>
+        <v>1.8104096000115533e-07</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B90" t="s">
         <v>5</v>
       </c>
       <c r="C90" s="1">
-        <v>8982.533203125</v>
+        <v>33684.73828125</v>
       </c>
       <c r="D90" s="2">
         <v>544681</v>
       </c>
       <c r="E90" s="1">
-        <v>4.554212118534906e-09</v>
+        <v>1.9129537065509794e-07</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B91" t="s">
         <v>5</v>
       </c>
       <c r="C91" s="1">
-        <v>1941.474365234375</v>
+        <v>33559.91015625</v>
       </c>
       <c r="D91" s="2">
         <v>544681</v>
       </c>
       <c r="E91" s="1">
-        <v>1.8386778766199541e-09</v>
+        <v>2.0914231413371454e-07</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B92" t="s">
         <v>5</v>
       </c>
       <c r="C92" s="1">
-        <v>1389.294921875</v>
+        <v>17296.1953125</v>
       </c>
       <c r="D92" s="2">
         <v>544681</v>
       </c>
       <c r="E92" s="1">
-        <v>9.4054630750406432e-10</v>
+        <v>1.8897863185429742e-07</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B93" t="s">
         <v>5</v>
       </c>
       <c r="C93" s="1">
-        <v>251.79917907714844</v>
+        <v>17406.576171875</v>
       </c>
       <c r="D93" s="2">
         <v>544681</v>
       </c>
       <c r="E93" s="1">
-        <v>2.4000823550807127e-10</v>
+        <v>1.9863198019720585e-07</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B94" t="s">
         <v>5</v>
       </c>
       <c r="C94" s="1">
-        <v>0</v>
+        <v>8982.533203125</v>
       </c>
       <c r="D94" s="2">
         <v>544681</v>
       </c>
       <c r="E94" s="1">
-        <v>0</v>
+        <v>1.2508341740158357e-07</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B95" t="s">
         <v>5</v>
       </c>
       <c r="C95" s="1">
-        <v>1.5880948305130005</v>
+        <v>1941.474365234375</v>
       </c>
       <c r="D95" s="2">
         <v>544681</v>
       </c>
       <c r="E95" s="1">
-        <v>3.2198824769652523e-12</v>
+        <v>5.0500084114446508e-08</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B96" t="s">
         <v>5</v>
       </c>
       <c r="C96" s="1">
-        <v>575.76568603515625</v>
+        <v>1389.294921875</v>
       </c>
       <c r="D96" s="2">
         <v>544681</v>
       </c>
       <c r="E96" s="1">
-        <v>1.1565025603843537e-09</v>
+        <v>2.5832514793933115e-08</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B97" t="s">
         <v>5</v>
       </c>
       <c r="C97" s="1">
-        <v>0</v>
+        <v>251.79917907714844</v>
       </c>
       <c r="D97" s="2">
         <v>544681</v>
       </c>
       <c r="E97" s="1">
-        <v>0</v>
+        <v>6.5919301128758434e-09</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B98" t="s">
         <v>5</v>
       </c>
       <c r="C98" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D98" s="2">
         <v>544681</v>
       </c>
       <c r="E98" s="1">
-        <v>0</v>
+        <v>2.5409620588168202e-11</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B99" t="s">
         <v>5</v>
       </c>
       <c r="C99" s="1">
-        <v>0</v>
+        <v>1.5880948305130005</v>
       </c>
       <c r="D99" s="2">
         <v>544681</v>
       </c>
       <c r="E99" s="1">
-        <v>0</v>
+        <v>8.8435474221437715e-11</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B100" t="s">
         <v>5</v>
       </c>
       <c r="C100" s="1">
-        <v>0</v>
+        <v>575.76568603515625</v>
       </c>
       <c r="D100" s="2">
         <v>544681</v>
       </c>
       <c r="E100" s="1">
-        <v>0</v>
+        <v>3.1763846664034645e-08</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B101" t="s">
         <v>5</v>
       </c>
       <c r="C101" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D101" s="2">
         <v>544681</v>
       </c>
       <c r="E101" s="1">
-        <v>0</v>
+        <v>1.201317517685041e-10</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B102" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C102" s="1">
-        <v>180.49602699279785</v>
+        <v>1</v>
       </c>
       <c r="D102" s="2">
-        <v>26646</v>
+        <v>544681</v>
       </c>
       <c r="E102" s="1">
-        <v>5.4552118378126124e-09</v>
+        <v>1.1864852156318051e-10</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B103" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C103" s="1">
-        <v>152.10235595703125</v>
+        <v>1</v>
       </c>
       <c r="D103" s="2">
-        <v>26646</v>
+        <v>544681</v>
       </c>
       <c r="E103" s="1">
-        <v>3.7452574375151926e-10</v>
+        <v>3.4642991253441835e-10</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B104" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C104" s="1">
-        <v>168.40696716308594</v>
+        <v>1</v>
       </c>
       <c r="D104" s="2">
-        <v>26646</v>
+        <v>544681</v>
       </c>
       <c r="E104" s="1">
-        <v>3.4450525765450379e-10</v>
+        <v>8.8253360175372109e-10</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B105" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C105" s="1">
-        <v>218.52995300292969</v>
+        <v>1</v>
       </c>
       <c r="D105" s="2">
-        <v>26646</v>
+        <v>544681</v>
       </c>
       <c r="E105" s="1">
-        <v>3.9474620794344162e-10</v>
+        <v>1.3238005136528841e-09</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B106" t="s">
         <v>6</v>
       </c>
       <c r="C106" s="1">
-        <v>391.04666137695313</v>
+        <v>180.49602699279785</v>
       </c>
       <c r="D106" s="2">
         <v>26646</v>
       </c>
       <c r="E106" s="1">
-        <v>1.8047557892586497e-09</v>
+        <v>1.4982975926614017e-07</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B107" t="s">
         <v>6</v>
       </c>
       <c r="C107" s="1">
-        <v>679.3365478515625</v>
+        <v>152.10235595703125</v>
       </c>
       <c r="D107" s="2">
         <v>26646</v>
       </c>
       <c r="E107" s="1">
-        <v>3.2621954026978983e-09</v>
+        <v>1.0286512086565835e-08</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B108" t="s">
         <v>6</v>
       </c>
       <c r="C108" s="1">
-        <v>428.40313720703125</v>
+        <v>168.40696716308594</v>
       </c>
       <c r="D108" s="2">
         <v>26646</v>
       </c>
       <c r="E108" s="1">
-        <v>2.7792592671715965e-09</v>
+        <v>9.4619867496703591e-09</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B109" t="s">
         <v>6</v>
       </c>
       <c r="C109" s="1">
-        <v>231.57841491699219</v>
+        <v>218.52995300292969</v>
       </c>
       <c r="D109" s="2">
         <v>26646</v>
       </c>
       <c r="E109" s="1">
-        <v>1.1168027613805975e-09</v>
+        <v>1.0841876729728028e-08</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B110" t="s">
         <v>6</v>
       </c>
       <c r="C110" s="1">
-        <v>95.509941101074219</v>
+        <v>391.04666137695313</v>
       </c>
       <c r="D110" s="2">
         <v>26646</v>
       </c>
       <c r="E110" s="1">
-        <v>3.428540229499788e-10</v>
+        <v>4.9568402715749471e-08</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B111" t="s">
         <v>6</v>
       </c>
       <c r="C111" s="1">
-        <v>12171.7392578125</v>
+        <v>679.3365478515625</v>
       </c>
       <c r="D111" s="2">
         <v>26646</v>
       </c>
       <c r="E111" s="1">
-        <v>2.5158589878060411e-08</v>
+        <v>8.959761288451773e-08</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B112" t="s">
         <v>6</v>
       </c>
       <c r="C112" s="1">
-        <v>6289.10595703125</v>
+        <v>428.40313720703125</v>
       </c>
       <c r="D112" s="2">
         <v>26646</v>
       </c>
       <c r="E112" s="1">
-        <v>2.6581771450651104e-08</v>
+        <v>7.6333563470143417e-08</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B113" t="s">
         <v>6</v>
       </c>
       <c r="C113" s="1">
-        <v>6330.93896484375</v>
+        <v>231.57841491699219</v>
       </c>
       <c r="D113" s="2">
         <v>26646</v>
       </c>
       <c r="E113" s="1">
-        <v>2.9363848241814594e-08</v>
+        <v>3.0673472650732947e-08</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B114" t="s">
         <v>6</v>
       </c>
       <c r="C114" s="1">
-        <v>3262.856201171875</v>
+        <v>95.509941101074219</v>
       </c>
       <c r="D114" s="2">
         <v>26646</v>
       </c>
       <c r="E114" s="1">
-        <v>2.6532841701509824e-08</v>
+        <v>9.4166345832036313e-09</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B115" t="s">
         <v>6</v>
       </c>
       <c r="C115" s="1">
-        <v>3283.679443359375</v>
+        <v>12171.7392578125</v>
       </c>
       <c r="D115" s="2">
         <v>26646</v>
       </c>
       <c r="E115" s="1">
-        <v>2.78881877591175e-08</v>
+        <v>6.9099161237318185e-07</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B116" t="s">
         <v>6</v>
       </c>
       <c r="C116" s="1">
-        <v>1694.51806640625</v>
+        <v>6289.10595703125</v>
       </c>
       <c r="D116" s="2">
         <v>26646</v>
       </c>
       <c r="E116" s="1">
-        <v>1.7561873733029643e-08</v>
+        <v>7.3007987566597876e-07</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B117" t="s">
         <v>6</v>
       </c>
       <c r="C117" s="1">
-        <v>366.25119018554688</v>
+        <v>6330.93896484375</v>
       </c>
       <c r="D117" s="2">
         <v>26646</v>
       </c>
       <c r="E117" s="1">
-        <v>7.090277254206967e-09</v>
+        <v>8.0649090250517474e-07</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B118" t="s">
         <v>6</v>
       </c>
       <c r="C118" s="1">
-        <v>262.08477783203125</v>
+        <v>3262.856201171875</v>
       </c>
       <c r="D118" s="2">
         <v>26646</v>
       </c>
       <c r="E118" s="1">
-        <v>3.6269180991865824e-09</v>
+        <v>7.287360404006904e-07</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B119" t="s">
         <v>6</v>
       </c>
       <c r="C119" s="1">
-        <v>47.500885009765625</v>
+        <v>3283.679443359375</v>
       </c>
       <c r="D119" s="2">
         <v>26646</v>
       </c>
       <c r="E119" s="1">
-        <v>9.2551555308517663e-10</v>
+        <v>7.6596120379690547e-07</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B120" t="s">
         <v>6</v>
       </c>
       <c r="C120" s="1">
-        <v>0</v>
+        <v>1694.51806640625</v>
       </c>
       <c r="D120" s="2">
         <v>26646</v>
       </c>
       <c r="E120" s="1">
-        <v>0</v>
+        <v>4.8234448968287325e-07</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B121" t="s">
         <v>6</v>
       </c>
       <c r="C121" s="1">
-        <v>0.29958760738372803</v>
+        <v>366.25119018554688</v>
       </c>
       <c r="D121" s="2">
         <v>26646</v>
       </c>
       <c r="E121" s="1">
-        <v>1.2416455884289856e-11</v>
+        <v>1.947375523059236e-07</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B122" t="s">
         <v>6</v>
       </c>
       <c r="C122" s="1">
-        <v>108.61583709716797</v>
+        <v>262.08477783203125</v>
       </c>
       <c r="D122" s="2">
         <v>26646</v>
       </c>
       <c r="E122" s="1">
-        <v>4.4596850656830611e-09</v>
+        <v>9.9614887005827768e-08</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B123" t="s">
         <v>6</v>
       </c>
       <c r="C123" s="1">
-        <v>0</v>
+        <v>47.500885009765625</v>
       </c>
       <c r="D123" s="2">
         <v>26646</v>
       </c>
       <c r="E123" s="1">
-        <v>0</v>
+        <v>2.5419685911742818e-08</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B124" t="s">
         <v>6</v>
       </c>
       <c r="C124" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D124" s="2">
         <v>26646</v>
       </c>
       <c r="E124" s="1">
-        <v>0</v>
+        <v>5.1940768353020417e-10</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B125" t="s">
         <v>6</v>
       </c>
       <c r="C125" s="1">
-        <v>0</v>
+        <v>0.29958760738372803</v>
       </c>
       <c r="D125" s="2">
         <v>26646</v>
       </c>
       <c r="E125" s="1">
-        <v>0</v>
+        <v>3.4102334844909876e-10</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B126" t="s">
         <v>6</v>
       </c>
       <c r="C126" s="1">
-        <v>0</v>
+        <v>108.61583709716797</v>
       </c>
       <c r="D126" s="2">
         <v>26646</v>
       </c>
       <c r="E126" s="1">
-        <v>0</v>
+        <v>1.2248719372109917e-07</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B127" t="s">
         <v>6</v>
       </c>
       <c r="C127" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D127" s="2">
         <v>26646</v>
       </c>
       <c r="E127" s="1">
-        <v>0</v>
+        <v>2.4556585653812135e-09</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1">
+        <v>28</v>
+      </c>
+      <c r="B128" t="s">
         <v>6</v>
       </c>
-      <c r="B128" t="s">
-        <v>7</v>
-      </c>
       <c r="C128" s="1">
-        <v>13443.02294921875</v>
+        <v>1</v>
       </c>
       <c r="D128" s="2">
-        <v>4579196</v>
+        <v>26646</v>
       </c>
       <c r="E128" s="1">
-        <v>2.3641972823895685e-09</v>
+        <v>2.4253394848017251e-09</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B129" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C129" s="1">
-        <v>9091.7099609375</v>
+        <v>1</v>
       </c>
       <c r="D129" s="2">
-        <v>4579196</v>
+        <v>26646</v>
       </c>
       <c r="E129" s="1">
-        <v>1.3026690837136812e-10</v>
+        <v>7.0815056041340085e-09</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B130" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C130" s="1">
-        <v>18183.419921875</v>
+        <v>1</v>
       </c>
       <c r="D130" s="2">
-        <v>4579196</v>
+        <v>26646</v>
       </c>
       <c r="E130" s="1">
-        <v>2.1644828984701547e-10</v>
+        <v>1.8040203997315984e-08</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B131" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C131" s="1">
-        <v>68187.8203125</v>
+        <v>1</v>
       </c>
       <c r="D131" s="2">
-        <v>4579196</v>
+        <v>26646</v>
       </c>
       <c r="E131" s="1">
-        <v>7.1673167401087312e-10</v>
+        <v>2.7060307772330816e-08</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B132" t="s">
         <v>7</v>
       </c>
       <c r="C132" s="1">
-        <v>388670.59375</v>
+        <v>13443.02294921875</v>
       </c>
       <c r="D132" s="2">
         <v>4579196</v>
       </c>
       <c r="E132" s="1">
-        <v>1.0437928743556313e-08</v>
+        <v>1.2946517635725741e-08</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B133" t="s">
         <v>7</v>
       </c>
       <c r="C133" s="1">
-        <v>892014.625</v>
+        <v>9091.7099609375</v>
       </c>
       <c r="D133" s="2">
         <v>4579196</v>
       </c>
       <c r="E133" s="1">
-        <v>2.4925263630848349e-08</v>
+        <v>7.1335115592319198e-10</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B134" t="s">
         <v>7</v>
       </c>
       <c r="C134" s="1">
-        <v>1672874.625</v>
+        <v>18183.419921875</v>
       </c>
       <c r="D134" s="2">
         <v>4579196</v>
       </c>
       <c r="E134" s="1">
-        <v>6.3151347262646595e-08</v>
+        <v>1.1852867576322978e-09</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B135" t="s">
         <v>7</v>
       </c>
       <c r="C135" s="1">
-        <v>1722879.25</v>
+        <v>68187.8203125</v>
       </c>
       <c r="D135" s="2">
         <v>4579196</v>
       </c>
       <c r="E135" s="1">
-        <v>4.8347725822850407e-08</v>
+        <v>3.9248755356879883e-09</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B136" t="s">
         <v>7</v>
       </c>
       <c r="C136" s="1">
-        <v>2179945.75</v>
+        <v>388670.59375</v>
       </c>
       <c r="D136" s="2">
         <v>4579196</v>
       </c>
       <c r="E136" s="1">
-        <v>4.553539767471193e-08</v>
+        <v>5.715886786106239e-08</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="1">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B137" t="s">
         <v>7</v>
       </c>
       <c r="C137" s="1">
-        <v>2146865</v>
+        <v>892014.625</v>
       </c>
       <c r="D137" s="2">
         <v>4579196</v>
       </c>
       <c r="E137" s="1">
-        <v>2.5821483617960439e-08</v>
+        <v>1.3649257368797407e-07</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B138" t="s">
         <v>7</v>
       </c>
       <c r="C138" s="1">
-        <v>2126356.5</v>
+        <v>1672874.625</v>
       </c>
       <c r="D138" s="2">
         <v>4579196</v>
       </c>
       <c r="E138" s="1">
-        <v>5.2296648789251776e-08</v>
+        <v>3.4582140528982563e-07</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B139" t="s">
         <v>7</v>
       </c>
       <c r="C139" s="1">
-        <v>1803709.375</v>
+        <v>1722879.25</v>
       </c>
       <c r="D139" s="2">
         <v>4579196</v>
       </c>
       <c r="E139" s="1">
-        <v>4.8680409037160643e-08</v>
+        <v>2.6475569825379353e-07</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="1">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B140" t="s">
         <v>7</v>
       </c>
       <c r="C140" s="1">
-        <v>557451.125</v>
+        <v>2179945.75</v>
       </c>
       <c r="D140" s="2">
         <v>4579196</v>
       </c>
       <c r="E140" s="1">
-        <v>2.6377609430028315e-08</v>
+        <v>2.493551960469631e-07</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="1">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B141" t="s">
         <v>7</v>
       </c>
       <c r="C141" s="1">
-        <v>222423.40625</v>
+        <v>2146865</v>
       </c>
       <c r="D141" s="2">
         <v>4579196</v>
       </c>
       <c r="E141" s="1">
-        <v>1.099215474198445e-08</v>
+        <v>1.4140033499643323e-07</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B142" t="s">
         <v>7</v>
       </c>
       <c r="C142" s="1">
-        <v>130643.3671875</v>
+        <v>2126356.5</v>
       </c>
       <c r="D142" s="2">
         <v>4579196</v>
       </c>
       <c r="E142" s="1">
-        <v>7.8787039115013613e-09</v>
+        <v>2.8638029903049755e-07</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B143" t="s">
         <v>7</v>
       </c>
       <c r="C143" s="1">
-        <v>78947.546875</v>
+        <v>1803709.375</v>
       </c>
       <c r="D143" s="2">
         <v>4579196</v>
       </c>
       <c r="E143" s="1">
-        <v>8.8933544972746859e-09</v>
+        <v>2.6657747298486356e-07</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B144" t="s">
         <v>7</v>
       </c>
       <c r="C144" s="1">
-        <v>53178.76953125</v>
+        <v>557451.125</v>
       </c>
       <c r="D144" s="2">
         <v>4579196</v>
       </c>
       <c r="E144" s="1">
-        <v>4.2822994039681817e-09</v>
+        <v>1.4444572116190102e-07</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="1">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B145" t="s">
         <v>7</v>
       </c>
       <c r="C145" s="1">
-        <v>18301.86328125</v>
+        <v>222423.40625</v>
       </c>
       <c r="D145" s="2">
         <v>4579196</v>
       </c>
       <c r="E145" s="1">
-        <v>2.0750097196042816e-09</v>
+        <v>6.0193848128164973e-08</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="1">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B146" t="s">
         <v>7</v>
       </c>
       <c r="C146" s="1">
-        <v>33230.90625</v>
+        <v>130643.3671875</v>
       </c>
       <c r="D146" s="2">
         <v>4579196</v>
       </c>
       <c r="E146" s="1">
-        <v>3.6568477135290323e-09</v>
+        <v>4.3144360972746654e-08</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="1">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B147" t="s">
         <v>7</v>
       </c>
       <c r="C147" s="1">
-        <v>28838.1875</v>
+        <v>78947.546875</v>
       </c>
       <c r="D147" s="2">
         <v>4579196</v>
       </c>
       <c r="E147" s="1">
-        <v>6.9547985148687985e-09</v>
+        <v>4.8700663057843485e-08</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B148" t="s">
         <v>7</v>
       </c>
       <c r="C148" s="1">
-        <v>5879.18310546875</v>
+        <v>53178.76953125</v>
       </c>
       <c r="D148" s="2">
         <v>4579196</v>
       </c>
       <c r="E148" s="1">
-        <v>1.404658722670149e-09</v>
+        <v>2.3450185793194578e-08</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="1">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B149" t="s">
         <v>7</v>
       </c>
       <c r="C149" s="1">
-        <v>314.47021484375</v>
+        <v>18301.86328125</v>
       </c>
       <c r="D149" s="2">
         <v>4579196</v>
       </c>
       <c r="E149" s="1">
-        <v>1.6360772459034223e-10</v>
+        <v>1.1362905283363034e-08</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="1">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B150" t="s">
         <v>7</v>
       </c>
       <c r="C150" s="1">
-        <v>0</v>
+        <v>33230.90625</v>
       </c>
       <c r="D150" s="2">
         <v>4579196</v>
       </c>
       <c r="E150" s="1">
-        <v>0</v>
+        <v>2.0025167302151203e-08</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="1">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B151" t="s">
         <v>7</v>
       </c>
       <c r="C151" s="1">
-        <v>1572.2359619140625</v>
+        <v>28838.1875</v>
       </c>
       <c r="D151" s="2">
         <v>4579196</v>
       </c>
       <c r="E151" s="1">
-        <v>2.3588462294554802e-09</v>
+        <v>3.8084987608044685e-08</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="1">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B152" t="s">
         <v>7</v>
       </c>
       <c r="C152" s="1">
-        <v>1662.5887451171875</v>
+        <v>5879.18310546875</v>
       </c>
       <c r="D152" s="2">
         <v>4579196</v>
       </c>
       <c r="E152" s="1">
-        <v>6.3545178008439507e-09</v>
+        <v>7.6920141367509132e-09</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="1">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B153" t="s">
         <v>7</v>
       </c>
       <c r="C153" s="1">
-        <v>1662.5887451171875</v>
+        <v>314.47021484375</v>
       </c>
       <c r="D153" s="2">
         <v>4579196</v>
       </c>
       <c r="E153" s="1">
-        <v>1.2709036489866321e-08</v>
+        <v>8.9592794294546252e-10</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="1">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B154" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C154" s="1">
-        <v>4344.2998046875</v>
+        <v>1</v>
       </c>
       <c r="D154" s="2">
-        <v>3474730</v>
+        <v>4579196</v>
       </c>
       <c r="E154" s="1">
-        <v>1.0068730293966155e-09</v>
+        <v>2.8138316329751056e-12</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="1">
+        <v>29</v>
+      </c>
+      <c r="B155" t="s">
         <v>7</v>
       </c>
-      <c r="B155" t="s">
-        <v>8</v>
-      </c>
       <c r="C155" s="1">
-        <v>20007.62109375</v>
+        <v>1572.2359619140625</v>
       </c>
       <c r="D155" s="2">
-        <v>3474730</v>
+        <v>4579196</v>
       </c>
       <c r="E155" s="1">
-        <v>3.7779146477845416e-10</v>
+        <v>1.2917215741481414e-08</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="1">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B156" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C156" s="1">
-        <v>28899.896484375</v>
+        <v>1662.5887451171875</v>
       </c>
       <c r="D156" s="2">
-        <v>3474730</v>
+        <v>4579196</v>
       </c>
       <c r="E156" s="1">
-        <v>4.5335984966143883e-10</v>
+        <v>3.4797807302311412e-08</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="1">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B157" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C157" s="1">
-        <v>46684.4453125</v>
+        <v>1662.5887451171875</v>
       </c>
       <c r="D157" s="2">
-        <v>3474730</v>
+        <v>4579196</v>
       </c>
       <c r="E157" s="1">
-        <v>6.4668109756027548e-10</v>
+        <v>5.2196710953467118e-08</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B158" t="s">
         <v>8</v>
       </c>
       <c r="C158" s="1">
-        <v>157837.875</v>
+        <v>4344.2998046875</v>
       </c>
       <c r="D158" s="2">
         <v>3474730</v>
       </c>
       <c r="E158" s="1">
-        <v>5.5861431036419162e-09</v>
+        <v>5.9955231890285177e-09</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B159" t="s">
         <v>8</v>
       </c>
       <c r="C159" s="1">
-        <v>549351.25</v>
+        <v>20007.62109375</v>
       </c>
       <c r="D159" s="2">
         <v>3474730</v>
       </c>
       <c r="E159" s="1">
-        <v>2.022954248559472e-08</v>
+        <v>2.2495960649848712e-09</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B160" t="s">
         <v>8</v>
       </c>
       <c r="C160" s="1">
-        <v>936842.6875</v>
+        <v>28899.896484375</v>
       </c>
       <c r="D160" s="2">
         <v>3474730</v>
       </c>
       <c r="E160" s="1">
-        <v>4.6607311787738581e-08</v>
+        <v>2.6995752300251752e-09</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="1">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B161" t="s">
         <v>8</v>
       </c>
       <c r="C161" s="1">
-        <v>1302913.375</v>
+        <v>46684.4453125</v>
       </c>
       <c r="D161" s="2">
         <v>3474730</v>
       </c>
       <c r="E161" s="1">
-        <v>4.8184229939352008e-08</v>
+        <v>3.8507255162301135e-09</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B162" t="s">
         <v>8</v>
       </c>
       <c r="C162" s="1">
-        <v>1570005.25</v>
+        <v>157837.875</v>
       </c>
       <c r="D162" s="2">
         <v>3474730</v>
       </c>
       <c r="E162" s="1">
-        <v>4.3218800982458561e-08</v>
+        <v>3.326323039232193e-08</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B163" t="s">
         <v>8</v>
       </c>
       <c r="C163" s="1">
-        <v>1674901.5</v>
+        <v>549351.25</v>
       </c>
       <c r="D163" s="2">
         <v>3474730</v>
       </c>
       <c r="E163" s="1">
-        <v>2.6548127252112863e-08</v>
+        <v>1.2045877895161539e-07</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B164" t="s">
         <v>8</v>
       </c>
       <c r="C164" s="1">
-        <v>1351896.875</v>
+        <v>936842.6875</v>
       </c>
       <c r="D164" s="2">
         <v>3474730</v>
       </c>
       <c r="E164" s="1">
-        <v>4.3817696138148676e-08</v>
+        <v>2.7752776077250019e-07</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B165" t="s">
         <v>8</v>
       </c>
       <c r="C165" s="1">
-        <v>856904.5625</v>
+        <v>1302913.375</v>
       </c>
       <c r="D165" s="2">
         <v>3474730</v>
       </c>
       <c r="E165" s="1">
-        <v>3.0478126689104101e-08</v>
+        <v>2.869176682906982e-07</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="1">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B166" t="s">
         <v>8</v>
       </c>
       <c r="C166" s="1">
-        <v>469480</v>
+        <v>1570005.25</v>
       </c>
       <c r="D166" s="2">
         <v>3474730</v>
       </c>
       <c r="E166" s="1">
-        <v>2.9276145951939725e-08</v>
+        <v>2.5735056397024891e-07</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="1">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B167" t="s">
         <v>8</v>
       </c>
       <c r="C167" s="1">
-        <v>165101.734375</v>
+        <v>1674901.5</v>
       </c>
       <c r="D167" s="2">
         <v>3474730</v>
       </c>
       <c r="E167" s="1">
-        <v>1.0752814638692598e-08</v>
+        <v>1.5808340947387478e-07</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="1">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B168" t="s">
         <v>8</v>
       </c>
       <c r="C168" s="1">
-        <v>96088.796875</v>
+        <v>1351896.875</v>
       </c>
       <c r="D168" s="2">
         <v>3474730</v>
       </c>
       <c r="E168" s="1">
-        <v>7.6367463464066532e-09</v>
+        <v>2.6091672111761e-07</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B169" t="s">
         <v>8</v>
       </c>
       <c r="C169" s="1">
-        <v>100041.7109375</v>
+        <v>856904.5625</v>
       </c>
       <c r="D169" s="2">
         <v>3474730</v>
       </c>
       <c r="E169" s="1">
-        <v>1.4851702978546655e-08</v>
+        <v>1.814849639458771e-07</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B170" t="s">
         <v>8</v>
       </c>
       <c r="C170" s="1">
-        <v>75425.0625</v>
+        <v>469480</v>
       </c>
       <c r="D170" s="2">
         <v>3474730</v>
       </c>
       <c r="E170" s="1">
-        <v>8.0042861227980211e-09</v>
+        <v>1.7432765275771089e-07</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="1">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B171" t="s">
         <v>8</v>
       </c>
       <c r="C171" s="1">
-        <v>54351.703125</v>
+        <v>165101.734375</v>
       </c>
       <c r="D171" s="2">
         <v>3474730</v>
       </c>
       <c r="E171" s="1">
-        <v>8.1209368119061764e-09</v>
+        <v>6.4028675694771664e-08</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="1">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B172" t="s">
         <v>8</v>
       </c>
       <c r="C172" s="1">
-        <v>30674.642578125</v>
+        <v>96088.796875</v>
       </c>
       <c r="D172" s="2">
         <v>3474730</v>
       </c>
       <c r="E172" s="1">
-        <v>4.4484873562566918e-09</v>
+        <v>4.5473743881530027e-08</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B173" t="s">
         <v>8</v>
       </c>
       <c r="C173" s="1">
-        <v>28858.61328125</v>
+        <v>100041.7109375</v>
       </c>
       <c r="D173" s="2">
         <v>3474730</v>
       </c>
       <c r="E173" s="1">
-        <v>9.1719192241157543e-09</v>
+        <v>8.8435903933259397e-08</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B174" t="s">
         <v>8</v>
       </c>
       <c r="C174" s="1">
-        <v>20119.1953125</v>
+        <v>75425.0625</v>
       </c>
       <c r="D174" s="2">
         <v>3474730</v>
       </c>
       <c r="E174" s="1">
-        <v>6.3347953549452996e-09</v>
+        <v>4.7662297220085748e-08</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="1">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B175" t="s">
         <v>8</v>
       </c>
       <c r="C175" s="1">
-        <v>10125.1298828125</v>
+        <v>54351.703125</v>
       </c>
       <c r="D175" s="2">
         <v>3474730</v>
       </c>
       <c r="E175" s="1">
-        <v>6.942135311049924e-09</v>
+        <v>4.8356906034996427e-08</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="1">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B176" t="s">
         <v>8</v>
       </c>
       <c r="C176" s="1">
-        <v>5227.9228515625</v>
+        <v>30674.642578125</v>
       </c>
       <c r="D176" s="2">
         <v>3474730</v>
       </c>
       <c r="E176" s="1">
-        <v>3.5401868103690504e-09</v>
+        <v>2.6488949700365083e-08</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="1">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B177" t="s">
         <v>8</v>
       </c>
       <c r="C177" s="1">
-        <v>1749.8079833984375</v>
+        <v>28858.61328125</v>
       </c>
       <c r="D177" s="2">
         <v>3474730</v>
       </c>
       <c r="E177" s="1">
-        <v>3.4597162912319845e-09</v>
+        <v>5.4615082234477086e-08</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="1">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B178" t="s">
         <v>8</v>
       </c>
       <c r="C178" s="1">
-        <v>3758.697998046875</v>
+        <v>20119.1953125</v>
       </c>
       <c r="D178" s="2">
         <v>3474730</v>
       </c>
       <c r="E178" s="1">
-        <v>1.8932299283846987e-08</v>
+        <v>3.7721154200198725e-08</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="1">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B179" t="s">
         <v>8</v>
       </c>
       <c r="C179" s="1">
-        <v>1381.36962890625</v>
+        <v>10125.1298828125</v>
       </c>
       <c r="D179" s="2">
         <v>3474730</v>
       </c>
       <c r="E179" s="1">
-        <v>1.3915725460833528e-08</v>
+        <v>4.1337617773251623e-08</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="1">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="B180" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C180" s="1">
-        <v>0</v>
+        <v>5227.9228515625</v>
       </c>
       <c r="D180" s="2">
-        <v>472523</v>
+        <v>3474730</v>
       </c>
       <c r="E180" s="1">
-        <v>0</v>
+        <v>2.1080387213601171e-08</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="1">
+        <v>29</v>
+      </c>
+      <c r="B181" t="s">
         <v>8</v>
       </c>
-      <c r="B181" t="s">
-        <v>9</v>
-      </c>
       <c r="C181" s="1">
-        <v>3634.8701171875</v>
+        <v>1749.8079833984375</v>
       </c>
       <c r="D181" s="2">
-        <v>472523</v>
+        <v>3474730</v>
       </c>
       <c r="E181" s="1">
-        <v>4.1930861560679489e-10</v>
+        <v>2.0601216732529792e-08</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="1">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="B182" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C182" s="1">
-        <v>10904.6103515625</v>
+        <v>3758.697998046875</v>
       </c>
       <c r="D182" s="2">
-        <v>472523</v>
+        <v>3474730</v>
       </c>
       <c r="E182" s="1">
-        <v>1.1107753605799076e-09</v>
+        <v>1.1273421307578246e-07</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="1">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B183" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C183" s="1">
-        <v>9692.9873046875</v>
+        <v>1381.36962890625</v>
       </c>
       <c r="D183" s="2">
-        <v>472523</v>
+        <v>3474730</v>
       </c>
       <c r="E183" s="1">
-        <v>2.5226476463302561e-09</v>
+        <v>6.2146902735094045e-08</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B184" t="s">
         <v>9</v>
       </c>
       <c r="C184" s="1">
-        <v>33925.453125</v>
+        <v>1</v>
       </c>
       <c r="D184" s="2">
         <v>472523</v>
       </c>
       <c r="E184" s="1">
-        <v>9.1867038420900826e-09</v>
+        <v>1.0148583362568075e-11</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="1">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B185" t="s">
         <v>9</v>
       </c>
       <c r="C185" s="1">
-        <v>100393</v>
+        <v>1</v>
       </c>
       <c r="D185" s="2">
         <v>472523</v>
       </c>
       <c r="E185" s="1">
-        <v>3.6727293206695322e-08</v>
+        <v>8.2681279357788018e-13</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="1">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B186" t="s">
         <v>9</v>
       </c>
       <c r="C186" s="1">
-        <v>134507.125</v>
+        <v>3634.8701171875</v>
       </c>
       <c r="D186" s="2">
         <v>472523</v>
       </c>
       <c r="E186" s="1">
-        <v>3.6579081097443122e-08</v>
+        <v>2.4968138667702533e-09</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="1">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B187" t="s">
         <v>9</v>
       </c>
       <c r="C187" s="1">
-        <v>144514.234375</v>
+        <v>10904.6103515625</v>
       </c>
       <c r="D187" s="2">
         <v>472523</v>
       </c>
       <c r="E187" s="1">
-        <v>2.9253669708850794e-08</v>
+        <v>6.6142198384966377e-09</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B188" t="s">
         <v>9</v>
       </c>
       <c r="C188" s="1">
-        <v>233576.234375</v>
+        <v>9692.9873046875</v>
       </c>
       <c r="D188" s="2">
         <v>472523</v>
       </c>
       <c r="E188" s="1">
-        <v>2.7225219412230217e-08</v>
+        <v>1.5021349497601477e-08</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="1">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B189" t="s">
         <v>9</v>
       </c>
       <c r="C189" s="1">
-        <v>243603.46875</v>
+        <v>33925.453125</v>
       </c>
       <c r="D189" s="2">
         <v>472523</v>
       </c>
       <c r="E189" s="1">
-        <v>5.8061406349452227e-08</v>
+        <v>5.4703122032151441e-08</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="1">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B190" t="s">
         <v>9</v>
       </c>
       <c r="C190" s="1">
-        <v>254660.453125</v>
+        <v>100393</v>
       </c>
       <c r="D190" s="2">
         <v>472523</v>
       </c>
       <c r="E190" s="1">
-        <v>6.6606318682715937e-08</v>
+        <v>2.186962291261807e-07</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="1">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B191" t="s">
         <v>9</v>
       </c>
       <c r="C191" s="1">
-        <v>107529.3984375</v>
+        <v>134507.125</v>
       </c>
       <c r="D191" s="2">
         <v>472523</v>
       </c>
       <c r="E191" s="1">
-        <v>4.9308539473713608e-08</v>
+        <v>2.1781367820494779e-07</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="1">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B192" t="s">
         <v>9</v>
       </c>
       <c r="C192" s="1">
-        <v>58113.5859375</v>
+        <v>144514.234375</v>
       </c>
       <c r="D192" s="2">
         <v>472523</v>
       </c>
       <c r="E192" s="1">
-        <v>2.783212060819551e-08</v>
+        <v>1.7419381492800312e-07</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="1">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B193" t="s">
         <v>9</v>
       </c>
       <c r="C193" s="1">
-        <v>67729.8125</v>
+        <v>233576.234375</v>
       </c>
       <c r="D193" s="2">
         <v>472523</v>
       </c>
       <c r="E193" s="1">
-        <v>3.9583444078061802e-08</v>
+        <v>1.6211521369768889e-07</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="1">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B194" t="s">
         <v>9</v>
       </c>
       <c r="C194" s="1">
-        <v>58950.8203125</v>
+        <v>243603.46875</v>
       </c>
       <c r="D194" s="2">
         <v>472523</v>
       </c>
       <c r="E194" s="1">
-        <v>6.4355120343861927e-08</v>
+        <v>3.4573227480905189e-07</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="1">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B195" t="s">
         <v>9</v>
       </c>
       <c r="C195" s="1">
-        <v>17435</v>
+        <v>254660.453125</v>
       </c>
       <c r="D195" s="2">
         <v>472523</v>
       </c>
       <c r="E195" s="1">
-        <v>1.3605890636370077e-08</v>
+        <v>3.9661378536948177e-07</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="1">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B196" t="s">
         <v>9</v>
       </c>
       <c r="C196" s="1">
-        <v>13030.740234375</v>
+        <v>107529.3984375</v>
       </c>
       <c r="D196" s="2">
         <v>472523</v>
       </c>
       <c r="E196" s="1">
-        <v>1.4317268259844695e-08</v>
+        <v>2.9361248721215816e-07</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="1">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B197" t="s">
         <v>9</v>
       </c>
       <c r="C197" s="1">
-        <v>17672.072265625</v>
+        <v>58113.5859375</v>
       </c>
       <c r="D197" s="2">
         <v>472523</v>
       </c>
       <c r="E197" s="1">
-        <v>1.8845968341452135e-08</v>
+        <v>1.6572906247347419e-07</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="1">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B198" t="s">
         <v>9</v>
       </c>
       <c r="C198" s="1">
-        <v>3065.32470703125</v>
+        <v>67729.8125</v>
       </c>
       <c r="D198" s="2">
         <v>472523</v>
       </c>
       <c r="E198" s="1">
-        <v>7.164062232334345e-09</v>
+        <v>2.3570345319967601e-07</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="1">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B199" t="s">
         <v>9</v>
       </c>
       <c r="C199" s="1">
-        <v>4138.96240234375</v>
+        <v>58950.8203125</v>
       </c>
       <c r="D199" s="2">
         <v>472523</v>
       </c>
       <c r="E199" s="1">
-        <v>9.5832231039594262e-09</v>
+        <v>3.8320879980346945e-07</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="1">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B200" t="s">
         <v>9</v>
       </c>
       <c r="C200" s="1">
-        <v>11138.72265625</v>
+        <v>17435</v>
       </c>
       <c r="D200" s="2">
         <v>472523</v>
       </c>
       <c r="E200" s="1">
-        <v>5.6159855432724726e-08</v>
+        <v>8.1017596187393792e-08</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="1">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B201" t="s">
         <v>9</v>
       </c>
       <c r="C201" s="1">
-        <v>575.0059814453125</v>
+        <v>13030.740234375</v>
       </c>
       <c r="D201" s="2">
         <v>472523</v>
       </c>
       <c r="E201" s="1">
-        <v>2.8633042603587455e-09</v>
+        <v>8.5253567760901205e-08</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="1">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B202" t="s">
         <v>9</v>
       </c>
       <c r="C202" s="1">
-        <v>4134.5166015625</v>
+        <v>17672.072265625</v>
       </c>
       <c r="D202" s="2">
         <v>472523</v>
       </c>
       <c r="E202" s="1">
-        <v>6.0113627853297658e-08</v>
+        <v>1.1222014251188739e-07</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="1">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B203" t="s">
         <v>9</v>
       </c>
       <c r="C203" s="1">
-        <v>16.977466583251953</v>
+        <v>3065.32470703125</v>
       </c>
       <c r="D203" s="2">
         <v>472523</v>
       </c>
       <c r="E203" s="1">
-        <v>6.2883531715129948e-10</v>
+        <v>4.2659102916786651e-08</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="1">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B204" t="s">
         <v>9</v>
       </c>
       <c r="C204" s="1">
-        <v>0</v>
+        <v>4138.96240234375</v>
       </c>
       <c r="D204" s="2">
         <v>472523</v>
       </c>
       <c r="E204" s="1">
-        <v>0</v>
+        <v>5.7064230674086502e-08</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="1">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B205" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C205" s="1">
-        <v>42157.80029296875</v>
+        <v>11138.72265625</v>
       </c>
       <c r="D205" s="2">
-        <v>785624</v>
+        <v>472523</v>
       </c>
       <c r="E205" s="1">
-        <v>4.3215464984314167e-08</v>
+        <v>3.3440929314565437e-07</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="B206" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C206" s="1">
-        <v>72246.0390625</v>
+        <v>575.0059814453125</v>
       </c>
       <c r="D206" s="2">
-        <v>785624</v>
+        <v>472523</v>
       </c>
       <c r="E206" s="1">
-        <v>6.0336073914868393e-09</v>
+        <v>1.7049822886860966e-08</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="1">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B207" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C207" s="1">
-        <v>79990.453125</v>
+        <v>4134.5166015625</v>
       </c>
       <c r="D207" s="2">
-        <v>785624</v>
+        <v>472523</v>
       </c>
       <c r="E207" s="1">
-        <v>5.5499778106593567e-09</v>
+        <v>3.5795244457403896e-07</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="1">
+        <v>30</v>
+      </c>
+      <c r="B208" t="s">
         <v>9</v>
       </c>
-      <c r="B208" t="s">
-        <v>10</v>
-      </c>
       <c r="C208" s="1">
-        <v>103798.0234375</v>
+        <v>16.977466583251953</v>
       </c>
       <c r="D208" s="2">
-        <v>785624</v>
+        <v>472523</v>
       </c>
       <c r="E208" s="1">
-        <v>6.3593592614097361e-09</v>
+        <v>3.7444607414727216e-09</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="1">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B209" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C209" s="1">
-        <v>185740.53125</v>
+        <v>1</v>
       </c>
       <c r="D209" s="2">
-        <v>785624</v>
+        <v>472523</v>
       </c>
       <c r="E209" s="1">
-        <v>2.9074605834011891e-08</v>
+        <v>3.3083213946127898e-10</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B210" t="s">
         <v>10</v>
       </c>
       <c r="C210" s="1">
-        <v>322673.34375</v>
+        <v>42157.80029296875</v>
       </c>
       <c r="D210" s="2">
         <v>785624</v>
       </c>
       <c r="E210" s="1">
-        <v>5.2553950524725224e-08</v>
+        <v>1.1869315130752511e-06</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B211" t="s">
         <v>10</v>
       </c>
       <c r="C211" s="1">
-        <v>203484.234375</v>
+        <v>72246.0390625</v>
       </c>
       <c r="D211" s="2">
         <v>785624</v>
       </c>
       <c r="E211" s="1">
-        <v>4.477385218137897e-08</v>
+        <v>1.6571564742662304e-07</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B212" t="s">
         <v>10</v>
       </c>
       <c r="C212" s="1">
-        <v>109995.8203125</v>
+        <v>79990.453125</v>
       </c>
       <c r="D212" s="2">
         <v>785624</v>
       </c>
       <c r="E212" s="1">
-        <v>1.7991686362961445e-08</v>
+        <v>1.52432548361503e-07</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B213" t="s">
         <v>10</v>
       </c>
       <c r="C213" s="1">
-        <v>89069.2734375</v>
+        <v>103798.0234375</v>
       </c>
       <c r="D213" s="2">
         <v>785624</v>
       </c>
       <c r="E213" s="1">
-        <v>1.0844408038224174e-08</v>
+        <v>1.7466257418163877e-07</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B214" t="s">
         <v>10</v>
       </c>
       <c r="C214" s="1">
-        <v>94129.8828125</v>
+        <v>185740.53125</v>
       </c>
       <c r="D214" s="2">
         <v>785624</v>
       </c>
       <c r="E214" s="1">
-        <v>6.5990053421671746e-09</v>
+        <v>7.9854669365886366e-07</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B215" t="s">
         <v>10</v>
       </c>
       <c r="C215" s="1">
-        <v>48507.75</v>
+        <v>322673.34375</v>
       </c>
       <c r="D215" s="2">
         <v>785624</v>
       </c>
       <c r="E215" s="1">
-        <v>6.9538192981610791e-09</v>
+        <v>1.4434170907406951e-06</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B216" t="s">
         <v>10</v>
       </c>
       <c r="C216" s="1">
-        <v>68175.4453125</v>
+        <v>203484.234375</v>
       </c>
       <c r="D216" s="2">
         <v>785624</v>
       </c>
       <c r="E216" s="1">
-        <v>1.0724822807617329e-08</v>
+        <v>1.2297333569222246e-06</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B217" t="s">
         <v>10</v>
       </c>
       <c r="C217" s="1">
-        <v>35136.44140625</v>
+        <v>109995.8203125</v>
       </c>
       <c r="D217" s="2">
         <v>785624</v>
       </c>
       <c r="E217" s="1">
-        <v>9.6908285840413555e-09</v>
+        <v>4.9414950353821041e-07</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B218" t="s">
         <v>10</v>
       </c>
       <c r="C218" s="1">
-        <v>35360.6796875</v>
+        <v>89069.2734375</v>
       </c>
       <c r="D218" s="2">
         <v>785624</v>
       </c>
       <c r="E218" s="1">
-        <v>1.0185853938082801e-08</v>
+        <v>2.9784638400087715e-07</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B219" t="s">
         <v>10</v>
       </c>
       <c r="C219" s="1">
-        <v>18247.61328125</v>
+        <v>94129.8828125</v>
       </c>
       <c r="D219" s="2">
         <v>785624</v>
       </c>
       <c r="E219" s="1">
-        <v>6.4142811062595229e-09</v>
+        <v>1.8124454470580531e-07</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B220" t="s">
         <v>10</v>
       </c>
       <c r="C220" s="1">
-        <v>3944.017822265625</v>
+        <v>48507.75</v>
       </c>
       <c r="D220" s="2">
         <v>785624</v>
       </c>
       <c r="E220" s="1">
-        <v>2.5896456090634956e-09</v>
+        <v>1.9098968095931923e-07</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B221" t="s">
         <v>10</v>
       </c>
       <c r="C221" s="1">
-        <v>2822.2900390625</v>
+        <v>68175.4453125</v>
       </c>
       <c r="D221" s="2">
         <v>785624</v>
       </c>
       <c r="E221" s="1">
-        <v>1.3246919117193556e-09</v>
+        <v>2.945619144156808e-07</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B222" t="s">
         <v>10</v>
       </c>
       <c r="C222" s="1">
-        <v>511.51873779296875</v>
+        <v>35136.44140625</v>
       </c>
       <c r="D222" s="2">
         <v>785624</v>
       </c>
       <c r="E222" s="1">
-        <v>3.3803435051105168e-10</v>
+        <v>2.6616280024427397e-07</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B223" t="s">
         <v>10</v>
       </c>
       <c r="C223" s="1">
-        <v>0</v>
+        <v>35360.6796875</v>
       </c>
       <c r="D223" s="2">
         <v>785624</v>
       </c>
       <c r="E223" s="1">
-        <v>0</v>
+        <v>2.7975889338449633e-07</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B224" t="s">
         <v>10</v>
       </c>
       <c r="C224" s="1">
-        <v>3.2261433601379395</v>
+        <v>18247.61328125</v>
       </c>
       <c r="D224" s="2">
         <v>785624</v>
       </c>
       <c r="E224" s="1">
-        <v>4.5349735251776213e-12</v>
+        <v>1.7617101377709332e-07</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B225" t="s">
         <v>10</v>
       </c>
       <c r="C225" s="1">
-        <v>1169.64208984375</v>
+        <v>3944.017822265625</v>
       </c>
       <c r="D225" s="2">
         <v>785624</v>
       </c>
       <c r="E225" s="1">
-        <v>1.6288508319917128e-09</v>
+        <v>7.1125739964372769e-08</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B226" t="s">
         <v>10</v>
       </c>
       <c r="C226" s="1">
-        <v>0</v>
+        <v>2822.2900390625</v>
       </c>
       <c r="D226" s="2">
         <v>785624</v>
       </c>
       <c r="E226" s="1">
-        <v>0</v>
+        <v>3.6383237755899245e-08</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B227" t="s">
         <v>10</v>
       </c>
       <c r="C227" s="1">
-        <v>0</v>
+        <v>511.51873779296875</v>
       </c>
       <c r="D227" s="2">
         <v>785624</v>
       </c>
       <c r="E227" s="1">
-        <v>0</v>
+        <v>9.2842604715315247e-09</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B228" t="s">
         <v>10</v>
       </c>
       <c r="C228" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D228" s="2">
         <v>785624</v>
       </c>
       <c r="E228" s="1">
-        <v>0</v>
+        <v>1.761674486844278e-11</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B229" t="s">
         <v>10</v>
       </c>
       <c r="C229" s="1">
-        <v>0</v>
+        <v>3.2261433601379395</v>
       </c>
       <c r="D229" s="2">
         <v>785624</v>
       </c>
       <c r="E229" s="1">
-        <v>0</v>
+        <v>1.245550190764888e-10</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B230" t="s">
         <v>10</v>
       </c>
       <c r="C230" s="1">
-        <v>0</v>
+        <v>1169.64208984375</v>
       </c>
       <c r="D230" s="2">
         <v>785624</v>
       </c>
       <c r="E230" s="1">
-        <v>0</v>
+        <v>4.47370958056581e-08</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="1">
+        <v>27</v>
+      </c>
+      <c r="B231" t="s">
+        <v>10</v>
+      </c>
+      <c r="C231" s="1">
+        <v>1</v>
+      </c>
+      <c r="D231" s="2">
+        <v>785624</v>
+      </c>
+      <c r="E231" s="1">
+        <v>8.3288542729320625e-11</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="1">
+        <v>28</v>
+      </c>
+      <c r="B232" t="s">
+        <v>10</v>
+      </c>
+      <c r="C232" s="1">
+        <v>1</v>
+      </c>
+      <c r="D232" s="2">
+        <v>785624</v>
+      </c>
+      <c r="E232" s="1">
+        <v>8.2260212530549381e-11</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="1">
+        <v>29</v>
+      </c>
+      <c r="B233" t="s">
+        <v>10</v>
+      </c>
+      <c r="C233" s="1">
+        <v>1</v>
+      </c>
+      <c r="D233" s="2">
+        <v>785624</v>
+      </c>
+      <c r="E233" s="1">
+        <v>2.4018334543463027e-10</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="1">
+        <v>30</v>
+      </c>
+      <c r="B234" t="s">
+        <v>10</v>
+      </c>
+      <c r="C234" s="1">
+        <v>1</v>
+      </c>
+      <c r="D234" s="2">
+        <v>785624</v>
+      </c>
+      <c r="E234" s="1">
+        <v>6.1186938848933892e-10</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="1">
+        <v>31</v>
+      </c>
+      <c r="B235" t="s">
+        <v>10</v>
+      </c>
+      <c r="C235" s="1">
+        <v>1</v>
+      </c>
+      <c r="D235" s="2">
+        <v>785624</v>
+      </c>
+      <c r="E235" s="1">
+        <v>9.1780416600073522e-10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>